<commit_message>
Conflict Resolution 3: Stuff that is Mine
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B88F949F-FCFA-46D6-B7C9-7C20D8C92B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62124753-205D-43C8-B248-F5E184CD29BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FC7A056-6ABF-45E9-A34A-00CAA2F99DB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Run 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>Sep</t>
   </si>
@@ -57,12 +58,21 @@
   <si>
     <t>Num</t>
   </si>
+  <si>
+    <t>Surviving</t>
+  </si>
+  <si>
+    <t>Average Height</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,16 +80,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,14 +109,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -406,16 +434,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF081DB-541A-4351-B730-BCB928942A1C}">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A31"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="6.77734375" customWidth="true"/>
+    <col min="9" max="9" width="2.15625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" style="1" customWidth="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -437,12 +470,969 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>6.5</v>
+      </c>
+      <c r="C2">
+        <v>-4</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>-21</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>-0.2</v>
+      </c>
+      <c r="H2">
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+      <c r="P2">
+        <v>-4</v>
+      </c>
+      <c r="Q2">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>-21</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+      <c r="T2">
+        <v>-0.2</v>
+      </c>
+      <c r="U2">
+        <v>0.2</v>
+      </c>
+      <c r="V2" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="W2" s="2">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.5</v>
+      </c>
+      <c r="C3">
+        <v>-4</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>-21</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>-0.2</v>
+      </c>
+      <c r="H3">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="0">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0">
+        <v>12.425338698271517</v>
+      </c>
+      <c r="O3">
+        <v>6.5</v>
+      </c>
+      <c r="P3">
+        <v>-4</v>
+      </c>
+      <c r="Q3">
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <v>-21</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>-0.2</v>
+      </c>
+      <c r="U3">
+        <v>0.2</v>
+      </c>
+      <c r="V3" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W3" s="2">
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6.5</v>
+      </c>
+      <c r="C4">
+        <v>-4</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>-21</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>-0.2</v>
+      </c>
+      <c r="H4">
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="0">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>6.5</v>
+      </c>
+      <c r="P4">
+        <v>-4</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>-21</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>-0.2</v>
+      </c>
+      <c r="U4">
+        <v>0.2</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1.71</v>
+      </c>
+      <c r="W4" s="2">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>6.5</v>
+      </c>
+      <c r="C5">
+        <v>-4</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>-21</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>-0.2</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="0">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0">
+        <v>5.388140932718505</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6.5</v>
+      </c>
+      <c r="C6">
+        <v>-4</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>-21</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>-0.2</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6.5</v>
+      </c>
+      <c r="C7">
+        <v>-4</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>-21</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>-0.2</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6.5</v>
+      </c>
+      <c r="C8">
+        <v>-4</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>-21</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>-0.2</v>
+      </c>
+      <c r="H8">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="0">
+        <v>1</v>
+      </c>
+      <c r="J8" s="0">
+        <v>10.907360706950234</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6.5</v>
+      </c>
+      <c r="C9">
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>-21</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>-0.2</v>
+      </c>
+      <c r="H9">
+        <v>0.2</v>
+      </c>
+      <c r="I9" s="0">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>6.5</v>
+      </c>
+      <c r="C10">
+        <v>-4</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>-21</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>-0.2</v>
+      </c>
+      <c r="H10">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="0">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6.5</v>
+      </c>
+      <c r="C11">
+        <v>-4</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>-21</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>-0.2</v>
+      </c>
+      <c r="H11">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="0">
+        <v>2</v>
+      </c>
+      <c r="J11" s="0">
+        <v>20.147379466159936</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6.5</v>
+      </c>
+      <c r="C12">
+        <v>-4</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>-21</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>-0.2</v>
+      </c>
+      <c r="H12">
+        <v>0.2</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6.5</v>
+      </c>
+      <c r="C13">
+        <v>-4</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>-21</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>-0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.2</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6.5</v>
+      </c>
+      <c r="C14">
+        <v>-4</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>-21</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>-0.2</v>
+      </c>
+      <c r="H14">
+        <v>0.2</v>
+      </c>
+      <c r="I14">
+        <v>18</v>
+      </c>
+      <c r="J14">
+        <v>168.20355809939352</v>
+      </c>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6.5</v>
+      </c>
+      <c r="C15">
+        <v>-4</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>-21</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>-0.2</v>
+      </c>
+      <c r="H15">
+        <v>0.2</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>184.53256025248658</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>6.5</v>
+      </c>
+      <c r="C16">
+        <v>-4</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>-21</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>-0.2</v>
+      </c>
+      <c r="H16">
+        <v>0.2</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>113.66890715630753</v>
+      </c>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6.5</v>
+      </c>
+      <c r="C17">
+        <v>-4</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>-21</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>-0.2</v>
+      </c>
+      <c r="H17">
+        <v>0.2</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>6.5</v>
+      </c>
+      <c r="C18">
+        <v>-4</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>-21</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>-0.2</v>
+      </c>
+      <c r="H18">
+        <v>0.2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>6.5</v>
+      </c>
+      <c r="C19">
+        <v>-4</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>-21</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>-0.2</v>
+      </c>
+      <c r="H19">
+        <v>0.2</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>19.356549911911106</v>
+      </c>
+    </row>
+    <row r="20" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>6.5</v>
+      </c>
+      <c r="C20">
+        <v>-4</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>-21</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>-0.2</v>
+      </c>
+      <c r="H20">
+        <v>0.2</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>6.5</v>
+      </c>
+      <c r="C21">
+        <v>-4</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>-21</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>-0.2</v>
+      </c>
+      <c r="H21">
+        <v>0.2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>6.5</v>
+      </c>
+      <c r="C22">
+        <v>-4</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>-21</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>-0.2</v>
+      </c>
+      <c r="H22">
+        <v>0.2</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>81.360035585494273</v>
+      </c>
+    </row>
+    <row r="23" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>6.5</v>
+      </c>
+      <c r="C23">
+        <v>-4</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>-21</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>-0.2</v>
+      </c>
+      <c r="H23">
+        <v>0.2</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>6.5</v>
+      </c>
+      <c r="C24">
+        <v>-4</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>-21</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>-0.2</v>
+      </c>
+      <c r="H24">
+        <v>0.2</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>6.4883022412949334</v>
+      </c>
+    </row>
+    <row r="25" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>6.5</v>
+      </c>
+      <c r="C25">
+        <v>-4</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>-21</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>-0.2</v>
+      </c>
+      <c r="H25">
+        <v>0.2</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>14.021805929859648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF081DB-541A-4351-B730-BCB928942A1C}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="8.77734375" customWidth="true"/>
+    <col min="9" max="9" width="11.6640625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>7</v>
       </c>
       <c r="C2">
@@ -460,8 +1450,14 @@
       <c r="G2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,8 +1479,14 @@
       <c r="G3">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -506,8 +1508,14 @@
       <c r="G4">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -529,8 +1537,14 @@
       <c r="G5">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -552,8 +1566,14 @@
       <c r="G6">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -575,8 +1595,14 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -598,8 +1624,14 @@
       <c r="G8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>7.5884519722368706</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -621,8 +1653,14 @@
       <c r="G9">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -644,8 +1682,14 @@
       <c r="G10">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>14.12841798433611</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -667,8 +1711,14 @@
       <c r="G11">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -690,8 +1740,14 @@
       <c r="G12">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>57.493057852881904</v>
+      </c>
+    </row>
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -713,8 +1769,14 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -736,8 +1798,14 @@
       <c r="G14">
         <v>-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>55.804506829739672</v>
+      </c>
+    </row>
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -759,8 +1827,14 @@
       <c r="G15">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -782,8 +1856,14 @@
       <c r="G16">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -805,8 +1885,14 @@
       <c r="G17">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -828,8 +1914,14 @@
       <c r="G18">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>67.672545269470248</v>
+      </c>
+    </row>
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -851,8 +1943,14 @@
       <c r="G19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -874,8 +1972,14 @@
       <c r="G20">
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>57.740155568967531</v>
+      </c>
+    </row>
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -897,8 +2001,14 @@
       <c r="G21">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>22.643175158486237</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -920,8 +2030,14 @@
       <c r="G22">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -943,8 +2059,14 @@
       <c r="G23">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>2.1369478109435907</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -966,8 +2088,14 @@
       <c r="G24">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -989,8 +2117,14 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>43.496043074433615</v>
+      </c>
+    </row>
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1012,8 +2146,14 @@
       <c r="G26">
         <v>-1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1035,8 +2175,14 @@
       <c r="G27">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>32.032765825950221</v>
+      </c>
+    </row>
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1058,8 +2204,14 @@
       <c r="G28">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>3.1622320797619392</v>
+      </c>
+    </row>
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1081,8 +2233,14 @@
       <c r="G29">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1104,8 +2262,14 @@
       <c r="G30">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>34.413155141176063</v>
+      </c>
+    </row>
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1126,6 +2290,12 @@
       </c>
       <c r="G31">
         <v>0</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>43.886464179128247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest edition that has good survival rates
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62124753-205D-43C8-B248-F5E184CD29BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9E38C2-D0A4-4F94-8A70-A316EC4F3A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="30 Minutes" sheetId="2" r:id="rId1"/>
     <sheet name="Run 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Sep</t>
   </si>
@@ -67,12 +67,54 @@
   <si>
     <t>dt</t>
   </si>
+  <si>
+    <t>average of 40</t>
+  </si>
+  <si>
+    <t>WagTim</t>
+  </si>
+  <si>
+    <t>WagStr</t>
+  </si>
+  <si>
+    <t>pi/24</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>pi/60</t>
+  </si>
+  <si>
+    <t>1.27 million meter incident</t>
+  </si>
+  <si>
+    <t>WStr</t>
+  </si>
+  <si>
+    <t>Wtim</t>
+  </si>
+  <si>
+    <t>switched to KNN</t>
+  </si>
+  <si>
+    <t>N_Agents</t>
+  </si>
+  <si>
+    <t>changed what hIgn means</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +129,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +158,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -109,21 +172,129 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,20 +606,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="6.77734375" customWidth="true"/>
-    <col min="9" max="9" width="2.15625" customWidth="true"/>
-    <col min="10" max="10" width="11.7109375" style="1" customWidth="true"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="5" width="5.77734375" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="6.21875" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="5.5546875" customWidth="1"/>
+    <col min="17" max="17" width="6.44140625" customWidth="1"/>
+    <col min="18" max="18" width="5.77734375" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" customWidth="1"/>
+    <col min="20" max="20" width="4.5546875" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" customWidth="1"/>
+    <col min="23" max="23" width="7" customWidth="1"/>
+    <col min="24" max="24" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -474,910 +662,1607 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
       </c>
       <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
-        <v>3</v>
-      </c>
       <c r="S1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
         <v>5</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.3">
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>-21</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H2">
         <v>0.2</v>
       </c>
-      <c r="I2" s="0">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>7</v>
+      <c r="I2">
+        <f>PI()/60</f>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3">
+        <v>23</v>
+      </c>
+      <c r="M2" s="3">
+        <v>2049.8367232326914</v>
+      </c>
+      <c r="N2" s="5">
+        <f>M2*L2/40</f>
+        <v>1178.6561158587976</v>
       </c>
       <c r="P2">
-        <v>-4</v>
+        <v>7</v>
       </c>
       <c r="Q2">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="R2">
-        <v>-21</v>
+        <v>8</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>-21</v>
       </c>
       <c r="T2">
+        <v>3</v>
+      </c>
+      <c r="U2">
         <v>-0.2</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>0.2</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="2">
         <v>4.3</v>
       </c>
-      <c r="W2" s="2">
+      <c r="AA2" s="2">
         <v>97.3</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>-21</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H3">
         <v>0.2</v>
       </c>
-      <c r="I3" s="0">
-        <v>1</v>
-      </c>
-      <c r="J3" s="0">
-        <v>12.425338698271517</v>
-      </c>
-      <c r="O3">
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="0">PI()/60</f>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>40</v>
+      </c>
+      <c r="L3" s="3">
+        <v>6</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2940.9456412018353</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" ref="N3:N25" si="1">M3*L3/40</f>
+        <v>441.14184618027531</v>
+      </c>
+      <c r="P3">
         <v>6.5</v>
       </c>
-      <c r="P3">
-        <v>-4</v>
-      </c>
       <c r="Q3">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="R3">
-        <v>-21</v>
+        <v>8</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>-21</v>
       </c>
       <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
         <v>-0.2</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>0.2</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W3" s="2">
+      <c r="AA3" s="2">
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>-21</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>0.2</v>
       </c>
-      <c r="I4" s="0">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>40</v>
+      </c>
+      <c r="L4" s="3">
+        <v>12</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1072.8262208527285</v>
+      </c>
+      <c r="N4" s="5">
+        <f t="shared" si="1"/>
+        <v>321.84786625581853</v>
+      </c>
+      <c r="P4">
         <v>6.5</v>
       </c>
-      <c r="P4">
-        <v>-4</v>
-      </c>
       <c r="Q4">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="R4">
-        <v>-21</v>
+        <v>8</v>
       </c>
       <c r="S4">
-        <v>3</v>
+        <v>-21</v>
       </c>
       <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
         <v>-0.2</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.2</v>
       </c>
-      <c r="V4" s="2">
+      <c r="W4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y4">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="2">
         <v>1.71</v>
       </c>
-      <c r="W4" s="2">
+      <c r="AA4" s="2">
         <v>26.9</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>-21</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <v>0.2</v>
       </c>
-      <c r="I5" s="0">
-        <v>1</v>
-      </c>
-      <c r="J5" s="0">
-        <v>5.388140932718505</v>
-      </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-    </row>
-    <row r="6" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>40</v>
+      </c>
+      <c r="L5" s="3">
+        <v>13</v>
+      </c>
+      <c r="M5" s="3">
+        <v>954.84149804077856</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="1"/>
+        <v>310.32348686325304</v>
+      </c>
+      <c r="P5">
+        <v>6</v>
+      </c>
+      <c r="Q5">
+        <v>-4.5</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>-18</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <v>-0.2</v>
+      </c>
+      <c r="V5">
+        <v>0.2</v>
+      </c>
+      <c r="W5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Y5">
+        <v>40</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>192.7</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>-21</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H6">
         <v>0.2</v>
       </c>
-      <c r="I6" s="0">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-    </row>
-    <row r="7" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>40</v>
+      </c>
+      <c r="L6" s="3">
+        <v>16</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2239.0442653282571</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="1"/>
+        <v>895.61770613130284</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>-5</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>-18</v>
+      </c>
+      <c r="T6">
+        <v>10</v>
+      </c>
+      <c r="U6">
+        <v>-0.2</v>
+      </c>
+      <c r="V6">
+        <v>0.2</v>
+      </c>
+      <c r="W6" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6">
+        <v>6</v>
+      </c>
+      <c r="Y6">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6.5</v>
-      </c>
-      <c r="C7">
-        <v>-4</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>-4.5</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>-21</v>
       </c>
-      <c r="F7">
-        <v>3</v>
+      <c r="F7" s="8">
+        <v>5</v>
       </c>
       <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7" s="9">
+        <v>40</v>
+      </c>
+      <c r="L7" s="3">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1231.4193315329537</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="1"/>
+        <v>615.70966576647686</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>-4.5</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>-18</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="U7">
         <v>-0.2</v>
       </c>
-      <c r="H7">
+      <c r="V7">
         <v>0.2</v>
       </c>
-      <c r="I7" s="0">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-    </row>
-    <row r="8" x14ac:dyDescent="0.3">
+      <c r="W7" t="s">
+        <v>15</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
+      <c r="Y7">
+        <v>40</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>165</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>-21</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H8">
         <v>0.2</v>
       </c>
-      <c r="I8" s="0">
-        <v>1</v>
-      </c>
-      <c r="J8" s="0">
-        <v>10.907360706950234</v>
-      </c>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-    </row>
-    <row r="9" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>40</v>
+      </c>
+      <c r="L8" s="3">
+        <v>16</v>
+      </c>
+      <c r="M8" s="3">
+        <v>956.12389468048616</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="1"/>
+        <v>382.44955787219448</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>-4.5</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>-18</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="U8">
+        <v>-0.2</v>
+      </c>
+      <c r="V8">
+        <v>0.2</v>
+      </c>
+      <c r="W8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Y8">
+        <v>40</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>7.13</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>-21</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G9">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>0.2</v>
       </c>
-      <c r="I9" s="0">
-        <v>0</v>
-      </c>
-      <c r="J9" s="0">
-        <v>0</v>
-      </c>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-    </row>
-    <row r="10" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>40</v>
+      </c>
+      <c r="L9" s="3">
+        <v>24</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1671.3907079149374</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="1"/>
+        <v>1002.8344247489624</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>-21</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G10">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H10">
         <v>0.2</v>
       </c>
-      <c r="I10" s="0">
-        <v>0</v>
-      </c>
-      <c r="J10" s="0">
-        <v>0</v>
-      </c>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-    </row>
-    <row r="11" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>40</v>
+      </c>
+      <c r="L10" s="3">
+        <v>10</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1226.6597840403738</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" si="1"/>
+        <v>306.66494601009344</v>
+      </c>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>-21</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G11">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H11">
         <v>0.2</v>
       </c>
-      <c r="I11" s="0">
-        <v>2</v>
-      </c>
-      <c r="J11" s="0">
-        <v>20.147379466159936</v>
-      </c>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-    </row>
-    <row r="12" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11" s="3">
+        <v>28</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1622.8428025189369</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="1"/>
+        <v>1135.9899617632559</v>
+      </c>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>-21</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G12">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H12">
         <v>0.2</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-    </row>
-    <row r="13" x14ac:dyDescent="0.3">
-      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>40</v>
+      </c>
+      <c r="L12" s="3">
+        <v>8</v>
+      </c>
+      <c r="M12" s="3">
+        <v>2604.2118755955662</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="1"/>
+        <v>520.84237511911329</v>
+      </c>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>6.5</v>
-      </c>
-      <c r="C13">
-        <v>-4</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-4.5</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>-21</v>
       </c>
-      <c r="F13">
-        <v>3</v>
+      <c r="F13" s="8">
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>-0.2</v>
-      </c>
-      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="H13" s="8">
         <v>0.2</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-    </row>
-    <row r="14" x14ac:dyDescent="0.3">
-      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="K13" s="8">
+        <v>40</v>
+      </c>
+      <c r="L13" s="12">
+        <v>15</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2162.9367423300182</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" si="1"/>
+        <v>811.10127837375683</v>
+      </c>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>6.5</v>
-      </c>
-      <c r="C14">
-        <v>-4</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="10">
+        <v>-4.5</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>-21</v>
       </c>
-      <c r="F14">
-        <v>3</v>
+      <c r="F14" s="10">
+        <v>15</v>
       </c>
       <c r="G14">
-        <v>-0.2</v>
-      </c>
-      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="H14" s="10">
         <v>0.2</v>
       </c>
       <c r="I14">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14" s="10">
+        <v>40</v>
+      </c>
+      <c r="L14" s="11">
         <v>18</v>
       </c>
-      <c r="J14">
-        <v>168.20355809939352</v>
-      </c>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-    </row>
-    <row r="15" x14ac:dyDescent="0.3">
+      <c r="M14" s="3">
+        <v>1144.6198468126672</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" si="1"/>
+        <v>515.07893106570032</v>
+      </c>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <v>-21</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G15">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H15">
         <v>0.2</v>
       </c>
       <c r="I15">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J15">
-        <v>184.53256025248658</v>
-      </c>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-    </row>
-    <row r="16" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <v>40</v>
+      </c>
+      <c r="L15" s="3">
+        <v>8</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1815.6405228563274</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" si="1"/>
+        <v>363.12810457126545</v>
+      </c>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <v>-21</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G16">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H16">
         <v>0.2</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J16">
-        <v>113.66890715630753</v>
-      </c>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>40</v>
+      </c>
+      <c r="L16" s="3">
+        <v>14</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2521.755697231762</v>
+      </c>
+      <c r="N16" s="5">
+        <f t="shared" si="1"/>
+        <v>882.61449403111669</v>
+      </c>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>-21</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G17">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H17">
         <v>0.2</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>40</v>
+      </c>
+      <c r="L17" s="3">
+        <v>13</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2117.9378353595248</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" si="1"/>
+        <v>688.32979649184551</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>3</v>
+      </c>
+      <c r="S17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>-21</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G18">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H18">
         <v>0.2</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" x14ac:dyDescent="0.3">
-      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>40</v>
+      </c>
+      <c r="L18" s="3">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>691.78917141377087</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" si="1"/>
+        <v>51.884187856032817</v>
+      </c>
+      <c r="P18" s="3">
+        <f t="shared" ref="P18:P23" si="2">L2</f>
+        <v>23</v>
+      </c>
+      <c r="Q18" s="3">
+        <f t="shared" ref="Q18:Q23" si="3">L8</f>
+        <v>16</v>
+      </c>
+      <c r="R18" s="3">
+        <f t="shared" ref="R18:R23" si="4">L14</f>
         <v>18</v>
       </c>
+      <c r="S18" s="3">
+        <f t="shared" ref="S18:S23" si="5">L20</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
       <c r="B19">
-        <v>6.5</v>
-      </c>
-      <c r="C19">
-        <v>-4</v>
+        <v>4</v>
+      </c>
+      <c r="C19" s="8">
+        <v>-4.5</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>-21</v>
       </c>
-      <c r="F19">
-        <v>3</v>
+      <c r="F19" s="8">
+        <v>15</v>
       </c>
       <c r="G19">
-        <v>-0.2</v>
-      </c>
-      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="H19" s="8">
         <v>0.2</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J19">
-        <v>19.356549911911106</v>
-      </c>
-    </row>
-    <row r="20" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K19" s="9">
+        <v>40</v>
+      </c>
+      <c r="L19" s="3">
+        <v>22</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1635.8970372426286</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" si="1"/>
+        <v>899.74337048344569</v>
+      </c>
+      <c r="P19" s="3">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="R19" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="S19" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>-21</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G20">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H20">
         <v>0.2</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>40</v>
+      </c>
+      <c r="L20" s="3">
+        <v>4</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1003.7406207489176</v>
+      </c>
+      <c r="N20" s="5">
+        <f t="shared" si="1"/>
+        <v>100.37406207489177</v>
+      </c>
+      <c r="P20" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="R20" s="3">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="S20" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>-21</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G21">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H21">
         <v>0.2</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <v>40</v>
+      </c>
+      <c r="L21" s="3">
+        <v>3</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1337.2965949675374</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" si="1"/>
+        <v>100.29724462256532</v>
+      </c>
+      <c r="P21" s="3">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="R21" s="3">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="S21" s="3">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>-21</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G22">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H22">
         <v>0.2</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J22">
-        <v>81.360035585494273</v>
-      </c>
-    </row>
-    <row r="23" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K22">
+        <v>40</v>
+      </c>
+      <c r="L22" s="3">
+        <v>10</v>
+      </c>
+      <c r="M22" s="3">
+        <v>2438.3661610043023</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" si="1"/>
+        <v>609.59154025107557</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="R22" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E23">
         <v>-21</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G23">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H23">
         <v>0.2</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K23">
+        <v>40</v>
+      </c>
+      <c r="L23" s="3">
+        <v>9</v>
+      </c>
+      <c r="M23" s="3">
+        <v>2642.114848129007</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="1"/>
+        <v>594.47584082902654</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="R23" s="3">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="S23" s="3">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>-21</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G24">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H24">
         <v>0.2</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J24">
-        <v>6.4883022412949334</v>
-      </c>
-    </row>
-    <row r="25" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>40</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>676.2880951784648</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="1"/>
+        <v>50.721607138384861</v>
+      </c>
+      <c r="O24" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24">
+        <f>AVERAGE(P18:P23)</f>
+        <v>15</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ref="Q24:S24" si="6">AVERAGE(Q18:Q23)</f>
+        <v>16.833333333333332</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="6"/>
+        <v>8.1666666666666661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <v>-21</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G25">
-        <v>-0.2</v>
+        <v>100</v>
       </c>
       <c r="H25">
         <v>0.2</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="J25">
-        <v>14.021805929859648</v>
+        <v>6</v>
+      </c>
+      <c r="K25">
+        <v>40</v>
+      </c>
+      <c r="L25" s="3">
+        <v>20</v>
+      </c>
+      <c r="M25" s="3">
+        <v>1511.688485390411</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="1"/>
+        <v>755.84424269520548</v>
+      </c>
+      <c r="P25" s="7">
+        <v>40</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>40</v>
+      </c>
+      <c r="R25" s="7">
+        <v>40</v>
+      </c>
+      <c r="S25" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L26" s="6">
+        <f>AVERAGE(L2:L25)</f>
+        <v>13.25</v>
+      </c>
+      <c r="N26" s="4">
+        <f>AVERAGE(N2:N25)</f>
+        <v>563.96927721057739</v>
+      </c>
+      <c r="O26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26">
+        <f>100*P24/P25</f>
+        <v>37.5</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:S26" si="7">100*Q24/Q25</f>
+        <v>42.083333333333329</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="7"/>
+        <v>32.5</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="7"/>
+        <v>20.416666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -1395,11 +2280,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="8.77734375" customWidth="true"/>
-    <col min="9" max="9" width="11.6640625" customWidth="true"/>
+    <col min="8" max="8" width="8.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1428,7 +2313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1457,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1486,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1515,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1544,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1573,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1602,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1631,7 +2516,7 @@
         <v>7.5884519722368706</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1660,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1689,7 +2574,7 @@
         <v>14.12841798433611</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1718,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1747,7 +2632,7 @@
         <v>57.493057852881904</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1776,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1805,7 +2690,7 @@
         <v>55.804506829739672</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1834,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1863,7 +2748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1892,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1921,7 +2806,7 @@
         <v>67.672545269470248</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1950,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1979,7 +2864,7 @@
         <v>57.740155568967531</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2008,7 +2893,7 @@
         <v>22.643175158486237</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2037,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2066,7 +2951,7 @@
         <v>2.1369478109435907</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2095,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2124,7 +3009,7 @@
         <v>43.496043074433615</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2153,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2182,7 +3067,7 @@
         <v>32.032765825950221</v>
       </c>
     </row>
-    <row r="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2211,7 +3096,7 @@
         <v>3.1622320797619392</v>
       </c>
     </row>
-    <row r="29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2240,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2269,7 +3154,7 @@
         <v>34.413155141176063</v>
       </c>
     </row>
-    <row r="31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
MasterScript compatible with new thermal model
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9E38C2-D0A4-4F94-8A70-A316EC4F3A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF3C805-EB47-4F39-9718-6CE24B092A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="30 Minutes" sheetId="2" r:id="rId1"/>
     <sheet name="Run 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Sep</t>
   </si>
@@ -109,6 +109,12 @@
   <si>
     <t>Percent</t>
   </si>
+  <si>
+    <t>5-20</t>
+  </si>
+  <si>
+    <t>Changed Thermal Model</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -268,27 +274,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -608,35 +617,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="5" width="5.77734375" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="16" max="16" width="5.5546875" customWidth="1"/>
-    <col min="17" max="17" width="6.44140625" customWidth="1"/>
-    <col min="18" max="18" width="5.77734375" customWidth="1"/>
-    <col min="19" max="19" width="6.33203125" customWidth="1"/>
-    <col min="20" max="20" width="4.5546875" customWidth="1"/>
-    <col min="21" max="21" width="6" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" customWidth="1"/>
-    <col min="23" max="23" width="7" customWidth="1"/>
-    <col min="24" max="24" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="true"/>
+    <col min="2" max="2" width="5" customWidth="true"/>
+    <col min="3" max="5" width="5.77734375" customWidth="true"/>
+    <col min="6" max="6" width="5.88671875" customWidth="true"/>
+    <col min="7" max="7" width="6.33203125" customWidth="true"/>
+    <col min="8" max="8" width="4.6640625" customWidth="true"/>
+    <col min="9" max="9" width="10.21875" customWidth="true"/>
+    <col min="10" max="10" width="6.21875" customWidth="true"/>
+    <col min="12" max="12" width="8.26953125" customWidth="true"/>
+    <col min="13" max="13" width="13.37890625" style="1" customWidth="true"/>
+    <col min="14" max="14" width="9.6640625" customWidth="true"/>
+    <col min="16" max="16" width="5.5546875" customWidth="true"/>
+    <col min="17" max="17" width="6.44140625" customWidth="true"/>
+    <col min="18" max="18" width="5.77734375" customWidth="true"/>
+    <col min="19" max="19" width="6.33203125" customWidth="true"/>
+    <col min="20" max="20" width="7.33203125" customWidth="true"/>
+    <col min="21" max="21" width="6" customWidth="true"/>
+    <col min="22" max="22" width="4.6640625" customWidth="true"/>
+    <col min="23" max="23" width="7" customWidth="true"/>
+    <col min="24" max="24" width="7.21875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -716,30 +725,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>-4.5</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>-21</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
-      <c r="H2">
-        <v>0.2</v>
+      <c r="H2" s="4">
+        <v>0.05</v>
       </c>
       <c r="I2">
         <f>PI()/60</f>
@@ -752,14 +761,14 @@
         <v>40</v>
       </c>
       <c r="L2" s="3">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="M2" s="3">
-        <v>2049.8367232326914</v>
-      </c>
-      <c r="N2" s="5">
+        <v>727.59271260179935</v>
+      </c>
+      <c r="N2" s="13">
         <f>M2*L2/40</f>
-        <v>1178.6561158587976</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>7</v>
@@ -798,30 +807,30 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>-4.5</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>-21</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
-      <c r="H3">
-        <v>0.2</v>
+      <c r="H3" s="4">
+        <v>0.05</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I25" si="0">PI()/60</f>
@@ -833,15 +842,11 @@
       <c r="K3">
         <v>40</v>
       </c>
-      <c r="L3" s="3">
-        <v>6</v>
-      </c>
-      <c r="M3" s="3">
-        <v>2940.9456412018353</v>
-      </c>
-      <c r="N3" s="5">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="13">
         <f t="shared" ref="N3:N25" si="1">M3*L3/40</f>
-        <v>441.14184618027531</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>6.5</v>
@@ -880,12 +885,12 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>-4.5</v>
@@ -897,13 +902,13 @@
         <v>-21</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>100</v>
       </c>
-      <c r="H4">
-        <v>0.2</v>
+      <c r="H4" s="4">
+        <v>0.05</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -915,15 +920,11 @@
       <c r="K4">
         <v>40</v>
       </c>
-      <c r="L4" s="3">
-        <v>12</v>
-      </c>
-      <c r="M4" s="3">
-        <v>1072.8262208527285</v>
-      </c>
-      <c r="N4" s="5">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="13">
         <f t="shared" si="1"/>
-        <v>321.84786625581853</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>6.5</v>
@@ -962,30 +963,30 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>-4.5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>-21</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>100</v>
       </c>
-      <c r="H5">
-        <v>0.2</v>
+      <c r="H5" s="4">
+        <v>0.05</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
@@ -997,15 +998,11 @@
       <c r="K5">
         <v>40</v>
       </c>
-      <c r="L5" s="3">
-        <v>13</v>
-      </c>
-      <c r="M5" s="3">
-        <v>954.84149804077856</v>
-      </c>
-      <c r="N5" s="5">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="13">
         <f t="shared" si="1"/>
-        <v>310.32348686325304</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>6</v>
@@ -1047,30 +1044,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>-4.5</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>-21</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>100</v>
       </c>
-      <c r="H6">
-        <v>0.2</v>
+      <c r="H6" s="4">
+        <v>0.05</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
@@ -1082,15 +1079,11 @@
       <c r="K6">
         <v>40</v>
       </c>
-      <c r="L6" s="3">
-        <v>16</v>
-      </c>
-      <c r="M6" s="3">
-        <v>2239.0442653282571</v>
-      </c>
-      <c r="N6" s="5">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="13">
         <f t="shared" si="1"/>
-        <v>895.61770613130284</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>6</v>
@@ -1129,30 +1122,30 @@
         <v>106.4</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+    <row r="7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7">
         <v>-4.5</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>-21</v>
       </c>
-      <c r="F7" s="8">
-        <v>5</v>
+      <c r="F7">
+        <v>10</v>
       </c>
       <c r="G7">
         <v>100</v>
       </c>
-      <c r="H7" s="8">
-        <v>0.2</v>
+      <c r="H7" s="4">
+        <v>0.05</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -1161,18 +1154,14 @@
       <c r="J7">
         <v>6</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="7">
         <v>40</v>
       </c>
-      <c r="L7" s="3">
-        <v>20</v>
-      </c>
-      <c r="M7" s="3">
-        <v>1231.4193315329537</v>
-      </c>
-      <c r="N7" s="5">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="13">
         <f t="shared" si="1"/>
-        <v>615.70966576647686</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>6</v>
@@ -1214,50 +1203,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>-4.5</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>-21</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-      <c r="H8">
-        <v>0.2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
-      </c>
-      <c r="K8">
-        <v>40</v>
-      </c>
-      <c r="L8" s="3">
-        <v>16</v>
-      </c>
-      <c r="M8" s="3">
-        <v>956.12389468048616</v>
-      </c>
-      <c r="N8" s="5">
+      <c r="H8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="13">
         <f t="shared" si="1"/>
-        <v>382.44955787219448</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <v>6</v>
@@ -1296,437 +1251,200 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="H9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="Q9">
         <v>-4.5</v>
       </c>
-      <c r="D9">
+      <c r="R9">
         <v>3</v>
       </c>
-      <c r="E9">
-        <v>-21</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
+      <c r="S9">
+        <v>-21</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="U9">
         <v>100</v>
       </c>
-      <c r="H9">
+      <c r="V9">
         <v>0.2</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J9">
+      <c r="W9" t="s">
+        <v>15</v>
+      </c>
+      <c r="X9">
         <v>6</v>
       </c>
-      <c r="K9">
+      <c r="Y9">
         <v>40</v>
       </c>
-      <c r="L9" s="3">
-        <v>24</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1671.3907079149374</v>
-      </c>
-      <c r="N9" s="5">
-        <f t="shared" si="1"/>
-        <v>1002.8344247489624</v>
-      </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
+      <c r="Z9" s="2">
+        <v>13.25</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>564</v>
+      </c>
       <c r="AB9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
+      <c r="H10" s="4"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
         <v>-4.5</v>
       </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>-21</v>
-      </c>
-      <c r="F10">
+      <c r="R10">
+        <v>2</v>
+      </c>
+      <c r="S10">
+        <v>-21</v>
+      </c>
+      <c r="T10">
         <v>10</v>
       </c>
-      <c r="G10">
+      <c r="U10">
         <v>100</v>
       </c>
-      <c r="H10">
-        <v>0.2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J10">
+      <c r="V10" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="W10" t="s">
+        <v>15</v>
+      </c>
+      <c r="X10">
         <v>6</v>
       </c>
-      <c r="K10">
+      <c r="Y10">
         <v>40</v>
-      </c>
-      <c r="L10" s="3">
-        <v>10</v>
-      </c>
-      <c r="M10" s="3">
-        <v>1226.6597840403738</v>
-      </c>
-      <c r="N10" s="5">
-        <f t="shared" si="1"/>
-        <v>306.66494601009344</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AB10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>-4.5</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>-21</v>
-      </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-      <c r="H11">
-        <v>0.2</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J11">
-        <v>6</v>
-      </c>
-      <c r="K11">
-        <v>40</v>
-      </c>
-      <c r="L11" s="3">
-        <v>28</v>
-      </c>
-      <c r="M11" s="3">
-        <v>1622.8428025189369</v>
-      </c>
-      <c r="N11" s="5">
+      <c r="H11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="13">
         <f t="shared" si="1"/>
-        <v>1135.9899617632559</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>-4.5</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>-21</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>100</v>
-      </c>
-      <c r="H12">
-        <v>0.2</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J12">
-        <v>6</v>
-      </c>
-      <c r="K12">
-        <v>40</v>
-      </c>
-      <c r="L12" s="3">
-        <v>8</v>
-      </c>
-      <c r="M12" s="3">
-        <v>2604.2118755955662</v>
-      </c>
-      <c r="N12" s="5">
+      <c r="H12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="13">
         <f t="shared" si="1"/>
-        <v>520.84237511911329</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+    <row r="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" s="8">
-        <v>-4.5</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>-21</v>
-      </c>
-      <c r="F13" s="8">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>100</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J13">
-        <v>6</v>
-      </c>
-      <c r="K13" s="8">
-        <v>40</v>
-      </c>
-      <c r="L13" s="12">
-        <v>15</v>
-      </c>
-      <c r="M13" s="3">
-        <v>2162.9367423300182</v>
-      </c>
-      <c r="N13" s="5">
+      <c r="H13" s="4"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="13">
         <f t="shared" si="1"/>
-        <v>811.10127837375683</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+    <row r="14" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" s="10">
-        <v>-4.5</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>-21</v>
-      </c>
-      <c r="F14" s="10">
-        <v>15</v>
-      </c>
-      <c r="G14">
-        <v>100</v>
-      </c>
-      <c r="H14" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J14">
-        <v>6</v>
-      </c>
-      <c r="K14" s="10">
-        <v>40</v>
-      </c>
-      <c r="L14" s="11">
-        <v>18</v>
-      </c>
-      <c r="M14" s="3">
-        <v>1144.6198468126672</v>
-      </c>
-      <c r="N14" s="5">
+      <c r="H14" s="4"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="13">
         <f t="shared" si="1"/>
-        <v>515.07893106570032</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>-4.5</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>-21</v>
-      </c>
-      <c r="F15">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <v>100</v>
-      </c>
-      <c r="H15">
-        <v>0.2</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J15">
-        <v>6</v>
-      </c>
-      <c r="K15">
-        <v>40</v>
-      </c>
-      <c r="L15" s="3">
-        <v>8</v>
-      </c>
-      <c r="M15" s="3">
-        <v>1815.6405228563274</v>
-      </c>
-      <c r="N15" s="5">
+      <c r="H15" s="4"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="13">
         <f t="shared" si="1"/>
-        <v>363.12810457126545</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>-4.5</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>-21</v>
-      </c>
-      <c r="F16">
-        <v>15</v>
-      </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <v>0.2</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J16">
-        <v>6</v>
-      </c>
-      <c r="K16">
-        <v>40</v>
-      </c>
-      <c r="L16" s="3">
-        <v>14</v>
-      </c>
-      <c r="M16" s="3">
-        <v>2521.755697231762</v>
-      </c>
-      <c r="N16" s="5">
+      <c r="H16" s="4"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="13">
         <f t="shared" si="1"/>
-        <v>882.61449403111669</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>-4.5</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>-21</v>
-      </c>
-      <c r="F17">
-        <v>15</v>
-      </c>
-      <c r="G17">
-        <v>100</v>
-      </c>
-      <c r="H17">
-        <v>0.2</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J17">
-        <v>6</v>
-      </c>
-      <c r="K17">
-        <v>40</v>
-      </c>
-      <c r="L17" s="3">
-        <v>13</v>
-      </c>
-      <c r="M17" s="3">
-        <v>2117.9378353595248</v>
-      </c>
-      <c r="N17" s="5">
+      <c r="H17" s="4"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="13">
         <f t="shared" si="1"/>
-        <v>688.32979649184551</v>
+        <v>0</v>
       </c>
       <c r="P17">
         <v>1</v>
@@ -1741,528 +1459,257 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>-4.5</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>-21</v>
-      </c>
-      <c r="F18">
-        <v>15</v>
-      </c>
-      <c r="G18">
-        <v>100</v>
-      </c>
-      <c r="H18">
-        <v>0.2</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J18">
-        <v>6</v>
-      </c>
-      <c r="K18">
-        <v>40</v>
-      </c>
-      <c r="L18" s="3">
-        <v>3</v>
-      </c>
-      <c r="M18" s="3">
-        <v>691.78917141377087</v>
-      </c>
-      <c r="N18" s="5">
+      <c r="H18" s="4"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="13">
         <f t="shared" si="1"/>
-        <v>51.884187856032817</v>
+        <v>0</v>
       </c>
       <c r="P18" s="3">
         <f t="shared" ref="P18:P23" si="2">L2</f>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="3">
         <f t="shared" ref="Q18:Q23" si="3">L8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R18" s="3">
         <f t="shared" ref="R18:R23" si="4">L14</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="S18" s="3">
         <f t="shared" ref="S18:S23" si="5">L20</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19" s="8">
-        <v>-4.5</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19">
-        <v>-21</v>
-      </c>
-      <c r="F19" s="8">
-        <v>15</v>
-      </c>
-      <c r="G19">
-        <v>100</v>
-      </c>
-      <c r="H19" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J19">
-        <v>6</v>
-      </c>
-      <c r="K19" s="9">
-        <v>40</v>
-      </c>
-      <c r="L19" s="3">
-        <v>22</v>
-      </c>
-      <c r="M19" s="3">
-        <v>1635.8970372426286</v>
-      </c>
-      <c r="N19" s="5">
+      <c r="H19" s="4"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="13">
         <f t="shared" si="1"/>
-        <v>899.74337048344569</v>
+        <v>0</v>
       </c>
       <c r="P19" s="3">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="3">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="R19" s="3">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="S19" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>-4.5</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>-21</v>
-      </c>
-      <c r="F20">
-        <v>20</v>
-      </c>
-      <c r="G20">
-        <v>100</v>
-      </c>
-      <c r="H20">
-        <v>0.2</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J20">
-        <v>6</v>
-      </c>
-      <c r="K20">
-        <v>40</v>
-      </c>
-      <c r="L20" s="3">
-        <v>4</v>
-      </c>
-      <c r="M20" s="3">
-        <v>1003.7406207489176</v>
-      </c>
-      <c r="N20" s="5">
+      <c r="H20" s="4"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="13">
         <f t="shared" si="1"/>
-        <v>100.37406207489177</v>
+        <v>0</v>
       </c>
       <c r="P20" s="3">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="3">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R20" s="3">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="S20" s="3">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>-4.5</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>-21</v>
-      </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21">
-        <v>100</v>
-      </c>
-      <c r="H21">
-        <v>0.2</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J21">
-        <v>6</v>
-      </c>
-      <c r="K21">
-        <v>40</v>
-      </c>
-      <c r="L21" s="3">
-        <v>3</v>
-      </c>
-      <c r="M21" s="3">
-        <v>1337.2965949675374</v>
-      </c>
-      <c r="N21" s="5">
+      <c r="H21" s="4"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="13">
         <f t="shared" si="1"/>
-        <v>100.29724462256532</v>
+        <v>0</v>
       </c>
       <c r="P21" s="3">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="3">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="R21" s="3">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="S21" s="3">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>-4.5</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="E22">
-        <v>-21</v>
-      </c>
-      <c r="F22">
-        <v>20</v>
-      </c>
-      <c r="G22">
-        <v>100</v>
-      </c>
-      <c r="H22">
-        <v>0.2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J22">
-        <v>6</v>
-      </c>
-      <c r="K22">
-        <v>40</v>
-      </c>
-      <c r="L22" s="3">
-        <v>10</v>
-      </c>
-      <c r="M22" s="3">
-        <v>2438.3661610043023</v>
-      </c>
-      <c r="N22" s="5">
+      <c r="H22" s="4"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="13">
         <f t="shared" si="1"/>
-        <v>609.59154025107557</v>
+        <v>0</v>
       </c>
       <c r="P22" s="3">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="3">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R22" s="3">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S22" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23">
-        <v>-4.5</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>-21</v>
-      </c>
-      <c r="F23">
-        <v>20</v>
-      </c>
-      <c r="G23">
-        <v>100</v>
-      </c>
-      <c r="H23">
-        <v>0.2</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J23">
-        <v>6</v>
-      </c>
-      <c r="K23">
-        <v>40</v>
-      </c>
-      <c r="L23" s="3">
-        <v>9</v>
-      </c>
-      <c r="M23" s="3">
-        <v>2642.114848129007</v>
-      </c>
-      <c r="N23" s="5">
+      <c r="H23" s="4"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="13">
         <f t="shared" si="1"/>
-        <v>594.47584082902654</v>
+        <v>0</v>
       </c>
       <c r="P23" s="3">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="3">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R23" s="3">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="S23" s="3">
         <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>-4.5</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24">
-        <v>-21</v>
-      </c>
-      <c r="F24">
-        <v>20</v>
-      </c>
-      <c r="G24">
-        <v>100</v>
-      </c>
-      <c r="H24">
-        <v>0.2</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J24">
-        <v>6</v>
-      </c>
-      <c r="K24">
-        <v>40</v>
-      </c>
-      <c r="L24" s="3">
-        <v>3</v>
-      </c>
-      <c r="M24" s="3">
-        <v>676.2880951784648</v>
-      </c>
-      <c r="N24" s="5">
+      <c r="H24" s="4"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="13">
         <f t="shared" si="1"/>
-        <v>50.721607138384861</v>
+        <v>0</v>
       </c>
       <c r="O24" t="s">
         <v>22</v>
       </c>
       <c r="P24">
         <f>AVERAGE(P18:P23)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q24">
         <f t="shared" ref="Q24:S24" si="6">AVERAGE(Q18:Q23)</f>
-        <v>16.833333333333332</v>
+        <v>0</v>
       </c>
       <c r="R24">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <f t="shared" si="6"/>
-        <v>8.1666666666666661</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25">
-        <v>-4.5</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>-21</v>
-      </c>
-      <c r="F25">
-        <v>20</v>
-      </c>
-      <c r="G25">
-        <v>100</v>
-      </c>
-      <c r="H25">
-        <v>0.2</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J25">
-        <v>6</v>
-      </c>
-      <c r="K25">
+      <c r="H25" s="4"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="5">
         <v>40</v>
       </c>
-      <c r="L25" s="3">
-        <v>20</v>
-      </c>
-      <c r="M25" s="3">
-        <v>1511.688485390411</v>
-      </c>
-      <c r="N25" s="5">
-        <f t="shared" si="1"/>
-        <v>755.84424269520548</v>
-      </c>
-      <c r="P25" s="7">
+      <c r="Q25" s="5">
         <v>40</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="R25" s="5">
         <v>40</v>
       </c>
-      <c r="R25" s="7">
+      <c r="S25" s="5">
         <v>40</v>
       </c>
-      <c r="S25" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="L26" s="6">
+    </row>
+    <row r="26" x14ac:dyDescent="0.3">
+      <c r="L26" s="4" t="e">
         <f>AVERAGE(L2:L25)</f>
-        <v>13.25</v>
-      </c>
-      <c r="N26" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" s="12">
         <f>AVERAGE(N2:N25)</f>
-        <v>563.96927721057739</v>
+        <v>0</v>
       </c>
       <c r="O26" t="s">
         <v>23</v>
       </c>
       <c r="P26">
         <f>100*P24/P25</f>
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="Q26">
         <f t="shared" ref="Q26:S26" si="7">100*Q24/Q25</f>
-        <v>42.083333333333329</v>
+        <v>0</v>
       </c>
       <c r="R26">
         <f t="shared" si="7"/>
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="S26">
         <f t="shared" si="7"/>
-        <v>20.416666666666664</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2280,11 +1727,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" customWidth="true"/>
+    <col min="9" max="9" width="11.6640625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +1760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2342,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2371,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2400,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2429,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2458,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2487,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2516,7 +1963,7 @@
         <v>7.5884519722368706</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2545,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2574,7 +2021,7 @@
         <v>14.12841798433611</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2603,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2632,7 +2079,7 @@
         <v>57.493057852881904</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2661,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2690,7 +2137,7 @@
         <v>55.804506829739672</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2719,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2748,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2777,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2806,7 +2253,7 @@
         <v>67.672545269470248</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2835,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2864,7 +2311,7 @@
         <v>57.740155568967531</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2893,7 +2340,7 @@
         <v>22.643175158486237</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2922,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2951,7 +2398,7 @@
         <v>2.1369478109435907</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2980,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3009,7 +2456,7 @@
         <v>43.496043074433615</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3038,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3067,7 +2514,7 @@
         <v>32.032765825950221</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3096,7 +2543,7 @@
         <v>3.1622320797619392</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3125,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3154,7 +2601,7 @@
         <v>34.413155141176063</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Major update. Option for parallel computing
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF3C805-EB47-4F39-9718-6CE24B092A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A838F9D8-41A1-49BA-8C02-6AD0EA6A50DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="2676" yWindow="1344" windowWidth="16080" windowHeight="10896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="30 Minutes" sheetId="2" r:id="rId1"/>
     <sheet name="Run 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Log" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Sep</t>
   </si>
@@ -112,9 +113,6 @@
   <si>
     <t>5-20</t>
   </si>
-  <si>
-    <t>Changed Thermal Model</t>
-  </si>
 </sst>
 </file>
 
@@ -170,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -228,17 +226,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -274,30 +261,27 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="true"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -617,35 +601,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="true"/>
-    <col min="2" max="2" width="5" customWidth="true"/>
-    <col min="3" max="5" width="5.77734375" customWidth="true"/>
-    <col min="6" max="6" width="5.88671875" customWidth="true"/>
-    <col min="7" max="7" width="6.33203125" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.21875" customWidth="true"/>
-    <col min="10" max="10" width="6.21875" customWidth="true"/>
-    <col min="12" max="12" width="2.15625" customWidth="true"/>
-    <col min="13" max="13" width="11.7109375" style="1" customWidth="true"/>
-    <col min="14" max="14" width="9.6640625" customWidth="true"/>
-    <col min="16" max="16" width="5.5546875" customWidth="true"/>
-    <col min="17" max="17" width="6.44140625" customWidth="true"/>
-    <col min="18" max="18" width="5.77734375" customWidth="true"/>
-    <col min="19" max="19" width="6.33203125" customWidth="true"/>
-    <col min="20" max="20" width="7.33203125" customWidth="true"/>
-    <col min="21" max="21" width="6" customWidth="true"/>
-    <col min="22" max="22" width="4.6640625" customWidth="true"/>
-    <col min="23" max="23" width="7" customWidth="true"/>
-    <col min="24" max="24" width="7.21875" customWidth="true"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="5" width="5.77734375" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="6.21875" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="5.5546875" customWidth="1"/>
+    <col min="17" max="17" width="6.44140625" customWidth="1"/>
+    <col min="18" max="18" width="5.77734375" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" customWidth="1"/>
+    <col min="20" max="20" width="7.33203125" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" customWidth="1"/>
+    <col min="23" max="23" width="7" customWidth="1"/>
+    <col min="24" max="24" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -725,7 +709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -733,13 +717,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>-4.5</v>
+        <v>-8</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>-21</v>
+        <v>-18</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -747,24 +731,22 @@
       <c r="G2">
         <v>100</v>
       </c>
-      <c r="H2" s="4">
-        <v>0.05</v>
+      <c r="H2">
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <f>PI()/60</f>
-        <v>5.2359877559829883E-2</v>
+        <f>PI()/24</f>
+        <v>0.1308996938995747</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K2">
         <v>40</v>
       </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
+      <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <f>M2*L2/40</f>
         <v>0</v>
       </c>
@@ -805,49 +787,14 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>-4.5</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>-21</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I25" si="0">PI()/60</f>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
-      </c>
-      <c r="K3">
-        <v>40</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3">
-        <v>337.26856550777512</v>
-      </c>
-      <c r="N3" s="13">
-        <f t="shared" ref="N3:N25" si="1">M3*L3/40</f>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="12">
+        <f t="shared" ref="N3:N25" si="0">M3*L3/40</f>
         <v>0</v>
       </c>
       <c r="P3">
@@ -887,47 +834,14 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>-4.5</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>-21</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I4">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="12">
         <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>40</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
@@ -967,49 +881,14 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>-4.5</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>-21</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I5">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="12">
         <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J5">
-        <v>6</v>
-      </c>
-      <c r="K5">
-        <v>40</v>
-      </c>
-      <c r="L5" s="3">
-        <v>4</v>
-      </c>
-      <c r="M5" s="3">
-        <v>271.24252494746469</v>
-      </c>
-      <c r="N5" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5">
@@ -1052,47 +931,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>-4.5</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>-21</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I6">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="12">
         <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>40</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P6">
@@ -1132,49 +978,14 @@
         <v>106.4</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>-4.5</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>-21</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I7">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="12">
         <f t="shared" si="0"/>
-        <v>5.2359877559829883E-2</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
-      <c r="K7" s="7">
-        <v>40</v>
-      </c>
-      <c r="L7" s="3">
-        <v>2</v>
-      </c>
-      <c r="M7" s="3">
-        <v>1274.1785547950885</v>
-      </c>
-      <c r="N7" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7">
@@ -1217,15 +1028,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="H8" s="4"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="13">
-        <f t="shared" si="1"/>
+      <c r="N8" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P8">
@@ -1265,15 +1075,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="H9" s="4"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="13">
-        <f t="shared" si="1"/>
+      <c r="N9" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P9">
@@ -1288,7 +1097,7 @@
       <c r="S9">
         <v>-21</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="T9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="U9">
@@ -1316,148 +1125,105 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="H10" s="4"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>2</v>
-      </c>
-      <c r="Q10">
-        <v>-4.5</v>
-      </c>
-      <c r="R10">
-        <v>2</v>
-      </c>
-      <c r="S10">
-        <v>-21</v>
-      </c>
-      <c r="T10">
-        <v>10</v>
-      </c>
-      <c r="U10">
-        <v>100</v>
-      </c>
-      <c r="V10" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="W10" t="s">
-        <v>15</v>
-      </c>
-      <c r="X10">
-        <v>6</v>
-      </c>
-      <c r="Y10">
-        <v>40</v>
+      <c r="N10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
-      <c r="AB10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="H11" s="4"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="13">
-        <f t="shared" si="1"/>
+      <c r="N11" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="H12" s="4"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="13">
-        <f t="shared" si="1"/>
+      <c r="N12" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="13">
-        <f t="shared" si="1"/>
+      <c r="N13" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="13">
-        <f t="shared" si="1"/>
+      <c r="N14" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="H15" s="4"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="13">
-        <f t="shared" si="1"/>
+      <c r="N15" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="H16" s="4"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="13">
-        <f t="shared" si="1"/>
+      <c r="N16" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="H17" s="4"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="13">
-        <f t="shared" si="1"/>
+      <c r="N17" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P17">
@@ -1473,184 +1239,176 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="H18" s="4"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="13">
-        <f t="shared" si="1"/>
+      <c r="N18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" ref="P18:P23" si="2">L2</f>
+        <f t="shared" ref="P18:P23" si="1">L2</f>
         <v>0</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" ref="Q18:Q23" si="3">L8</f>
+        <f t="shared" ref="Q18:Q23" si="2">L8</f>
         <v>0</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" ref="R18:R23" si="4">L14</f>
+        <f t="shared" ref="R18:R23" si="3">L14</f>
         <v>0</v>
       </c>
       <c r="S18" s="3">
-        <f t="shared" ref="S18:S23" si="5">L20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" x14ac:dyDescent="0.3">
+        <f t="shared" ref="S18:S23" si="4">L20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="K19" s="7"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="13">
+      <c r="N19" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R19" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S19" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S19" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="H20" s="4"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="13">
+      <c r="N20" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P20" s="3">
+      <c r="Q20" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="R20" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R20" s="3">
+      <c r="S20" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S20" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="H21" s="4"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="13">
+      <c r="N21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q21" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="R21" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R21" s="3">
+      <c r="S21" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S21" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="H22" s="4"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="13">
+      <c r="N22" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P22" s="3">
+      <c r="Q22" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="R22" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R22" s="3">
+      <c r="S22" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S22" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="H23" s="4"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="13">
+      <c r="N23" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P23" s="3">
+      <c r="Q23" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="R23" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R23" s="3">
+      <c r="S23" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S23" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="H24" s="4"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="13">
-        <f t="shared" si="1"/>
+      <c r="N24" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O24" t="s">
@@ -1661,27 +1419,26 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" ref="Q24:S24" si="6">AVERAGE(Q18:Q23)</f>
+        <f t="shared" ref="Q24:S24" si="5">AVERAGE(Q18:Q23)</f>
         <v>0</v>
       </c>
       <c r="R24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="H25" s="4"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="13">
-        <f t="shared" si="1"/>
+      <c r="N25" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P25" s="5">
@@ -1697,12 +1454,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L26" s="4" t="e">
         <f>AVERAGE(L2:L25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="11">
         <f>AVERAGE(N2:N25)</f>
         <v>0</v>
       </c>
@@ -1714,15 +1471,15 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26:S26" si="7">100*Q24/Q25</f>
+        <f t="shared" ref="Q26:S26" si="6">100*Q24/Q25</f>
         <v>0</v>
       </c>
       <c r="R26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1741,11 +1498,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="8.77734375" customWidth="true"/>
-    <col min="9" max="9" width="11.6640625" customWidth="true"/>
+    <col min="8" max="8" width="8.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1774,7 +1531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1803,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1832,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1861,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1890,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1919,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1948,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1977,7 +1734,7 @@
         <v>7.5884519722368706</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2006,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2035,7 +1792,7 @@
         <v>14.12841798433611</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2064,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2093,7 +1850,7 @@
         <v>57.493057852881904</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2122,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2151,7 +1908,7 @@
         <v>55.804506829739672</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2180,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2209,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2238,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2267,7 +2024,7 @@
         <v>67.672545269470248</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2296,7 +2053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2325,7 +2082,7 @@
         <v>57.740155568967531</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2354,7 +2111,7 @@
         <v>22.643175158486237</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2383,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2412,7 +2169,7 @@
         <v>2.1369478109435907</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2441,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2470,7 +2227,7 @@
         <v>43.496043074433615</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2499,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2528,7 +2285,7 @@
         <v>32.032765825950221</v>
       </c>
     </row>
-    <row r="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2557,7 +2314,7 @@
         <v>3.1622320797619392</v>
       </c>
     </row>
-    <row r="29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2586,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2615,7 +2372,7 @@
         <v>34.413155141176063</v>
       </c>
     </row>
-    <row r="31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2647,4 +2404,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54043E1B-DEBB-41CB-BDB8-BC798E86B541}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Simplified acceleration arrows, added focused view
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4FA59E-2E34-493A-904D-E9B1753C0A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD705FE-2363-44BE-A536-1712D249D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Input (First Sheet Always)" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Log 06-28" sheetId="3" r:id="rId3"/>
     <sheet name="Log 06-29" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="214">
   <si>
     <t>Sep</t>
   </si>
@@ -638,6 +638,48 @@
   </si>
   <si>
     <t>13:50:28</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>14:15:16</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>14:18:12</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>14:21:17</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>14:57:26</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>21:05:27</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>21:25:29</t>
+  </si>
+  <si>
+    <t>06-29-22</t>
+  </si>
+  <si>
+    <t>21:36:57</t>
   </si>
 </sst>
 </file>
@@ -709,18 +751,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
+        <fgColor theme="7" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -780,35 +822,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="true"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyBorder="true"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="true"/>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="true"/>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="true"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -820,7 +864,7 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -830,14 +874,14 @@
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -845,7 +889,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="0">
+      <border outline="false">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -853,21 +897,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="0">
+      <border outline="false">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -877,14 +921,14 @@
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -892,7 +936,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="0">
+      <border outline="false">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -900,14 +944,14 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="0">
+      <border outline="false">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border outline="false">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
@@ -927,61 +971,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}" name="Table1" displayName="Table1" ref="A1:U73" totalsRowShown="0" headerRowCellStyle="Good" dataCellStyle="Good">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="1" name="Table1" displayName="Table1" ref="A1:U73" totalsRowShown="false" headerRowCellStyle="Good" dataCellStyle="Good" mc:Ignorable="xr xr3" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}">
   <autoFilter ref="A1:U73" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{CD2AE5F0-A067-48DC-945F-0570E6312B06}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{124F9F36-5D64-42C9-B806-47D006C6CA9A}" name="Time"/>
-    <tableColumn id="3" xr3:uid="{D7BF650C-D78F-47FF-A191-5F7C2A908175}" name="Separation" dataDxfId="13" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{63B5EB73-2B29-4135-ADE4-880D10883200}" name="Cohesion" dataDxfId="12" dataCellStyle="Input"/>
-    <tableColumn id="5" xr3:uid="{B9124B5C-D0AE-4010-BC14-B88C64B9756E}" name="Alignment" dataDxfId="11" dataCellStyle="Input"/>
-    <tableColumn id="6" xr3:uid="{BFB8E62F-AE8F-403E-92F6-61D4A7E19ADA}" name="Migration" dataDxfId="10" dataCellStyle="Input"/>
-    <tableColumn id="7" xr3:uid="{2936402B-09B3-4C5D-B402-9D28E0F2E8A8}" name="Height Priority" dataCellStyle="Input"/>
-    <tableColumn id="8" xr3:uid="{E7AEB934-FAB1-4B69-BE53-62A8F39A764C}" name="Height Ignore" dataDxfId="9" dataCellStyle="Input"/>
-    <tableColumn id="9" xr3:uid="{736093B2-EF64-4847-B7C4-2E9CDB164008}" name="dt" dataDxfId="8" dataCellStyle="Input"/>
-    <tableColumn id="10" xr3:uid="{C5795275-E854-4EFB-88B9-C49B37FF6999}" name="Waggle Strength" dataDxfId="7" dataCellStyle="Input"/>
-    <tableColumn id="11" xr3:uid="{A6DEE2DA-660A-4D68-987E-58E933151945}" name="Waggle Time" dataCellStyle="Input"/>
-    <tableColumn id="12" xr3:uid="{9FDB18DD-6007-41EC-9734-C49EC48B769A}" name="# of Agents" dataCellStyle="Input"/>
-    <tableColumn id="13" xr3:uid="{C6C801F0-B377-4F31-A463-104D29538A52}" name="Total Time" dataCellStyle="Input"/>
-    <tableColumn id="14" xr3:uid="{F01BD334-4E3B-408C-AA8F-9A18BE4AA0BD}" name="# of Thermals" dataCellStyle="Input"/>
-    <tableColumn id="15" xr3:uid="{2D9CAFF3-8B5B-409E-8F68-FBCE1BBB76DF}" name="Neighbor Radius" dataCellStyle="Input"/>
-    <tableColumn id="16" xr3:uid="{E107D01D-AB0E-4655-9B1A-B57B0C63EC40}" name="Neighbor Angle Range" dataCellStyle="Input"/>
-    <tableColumn id="17" xr3:uid="{91A8CDD3-26BE-4A07-A1A4-F64FB8CB0B40}" name="K" dataCellStyle="Input"/>
-    <tableColumn id="18" xr3:uid="{65DCF8D9-31A5-4CC2-87E2-88950F9548CF}" name="FOV" dataCellStyle="Input"/>
-    <tableColumn id="19" xr3:uid="{403513BC-6E74-4FB8-BBA8-258B934381A5}" name="Surviving" dataCellStyle="Good"/>
-    <tableColumn id="20" xr3:uid="{9C3C23D8-78A8-4FC2-B90D-4AAEA40043BA}" name="Average Z of survivors" dataCellStyle="Good"/>
-    <tableColumn id="21" xr3:uid="{D2031C1F-0DC7-4809-88C0-819C871DDDA0}" name="Flight Time" dataCellStyle="Good"/>
+    <tableColumn id="1" name="Date" xr3:uid="{CD2AE5F0-A067-48DC-945F-0570E6312B06}"/>
+    <tableColumn id="2" name="Time" xr3:uid="{124F9F36-5D64-42C9-B806-47D006C6CA9A}"/>
+    <tableColumn id="3" name="Separation" dataDxfId="13" dataCellStyle="Input" xr3:uid="{D7BF650C-D78F-47FF-A191-5F7C2A908175}"/>
+    <tableColumn id="4" name="Cohesion" dataDxfId="12" dataCellStyle="Input" xr3:uid="{63B5EB73-2B29-4135-ADE4-880D10883200}"/>
+    <tableColumn id="5" name="Alignment" dataDxfId="11" dataCellStyle="Input" xr3:uid="{B9124B5C-D0AE-4010-BC14-B88C64B9756E}"/>
+    <tableColumn id="6" name="Migration" dataDxfId="10" dataCellStyle="Input" xr3:uid="{BFB8E62F-AE8F-403E-92F6-61D4A7E19ADA}"/>
+    <tableColumn id="7" name="Height Priority" dataCellStyle="Input" xr3:uid="{2936402B-09B3-4C5D-B402-9D28E0F2E8A8}"/>
+    <tableColumn id="8" name="Height Ignore" dataDxfId="9" dataCellStyle="Input" xr3:uid="{E7AEB934-FAB1-4B69-BE53-62A8F39A764C}"/>
+    <tableColumn id="9" name="dt" dataDxfId="8" dataCellStyle="Input" xr3:uid="{736093B2-EF64-4847-B7C4-2E9CDB164008}"/>
+    <tableColumn id="10" name="Waggle Strength" dataDxfId="7" dataCellStyle="Input" xr3:uid="{C5795275-E854-4EFB-88B9-C49B37FF6999}"/>
+    <tableColumn id="11" name="Waggle Time" dataCellStyle="Input" xr3:uid="{A6DEE2DA-660A-4D68-987E-58E933151945}"/>
+    <tableColumn id="12" name="# of Agents" dataCellStyle="Input" xr3:uid="{9FDB18DD-6007-41EC-9734-C49EC48B769A}"/>
+    <tableColumn id="13" name="Total Time" dataCellStyle="Input" xr3:uid="{C6C801F0-B377-4F31-A463-104D29538A52}"/>
+    <tableColumn id="14" name="# of Thermals" dataCellStyle="Input" xr3:uid="{F01BD334-4E3B-408C-AA8F-9A18BE4AA0BD}"/>
+    <tableColumn id="15" name="Neighbor Radius" dataCellStyle="Input" xr3:uid="{2D9CAFF3-8B5B-409E-8F68-FBCE1BBB76DF}"/>
+    <tableColumn id="16" name="Neighbor Angle Range" dataCellStyle="Input" xr3:uid="{E107D01D-AB0E-4655-9B1A-B57B0C63EC40}"/>
+    <tableColumn id="17" name="K" dataCellStyle="Input" xr3:uid="{91A8CDD3-26BE-4A07-A1A4-F64FB8CB0B40}"/>
+    <tableColumn id="18" name="FOV" dataCellStyle="Input" xr3:uid="{65DCF8D9-31A5-4CC2-87E2-88950F9548CF}"/>
+    <tableColumn id="19" name="Surviving" dataCellStyle="Good" xr3:uid="{403513BC-6E74-4FB8-BBA8-258B934381A5}"/>
+    <tableColumn id="20" name="Average Z of survivors" dataCellStyle="Good" xr3:uid="{9C3C23D8-78A8-4FC2-B90D-4AAEA40043BA}"/>
+    <tableColumn id="21" name="Flight Time" dataCellStyle="Good" xr3:uid="{D2031C1F-0DC7-4809-88C0-819C871DDDA0}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C51EEC99-3A6C-45AC-AAA7-E48D93D343CE}" name="Table13" displayName="Table13" ref="A1:T73" totalsRowShown="0" headerRowCellStyle="Good" dataCellStyle="Good">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="2" name="Table13" displayName="Table13" ref="A1:T73" totalsRowShown="false" headerRowCellStyle="Good" dataCellStyle="Good" mc:Ignorable="xr xr3" xr:uid="{C51EEC99-3A6C-45AC-AAA7-E48D93D343CE}">
   <autoFilter ref="A1:T73" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{517919BE-7171-41C2-BD81-2BD8FD4BA9AB}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{32646A5F-2643-46B1-9978-5CED855C6BAA}" name="Time"/>
-    <tableColumn id="3" xr3:uid="{C0D106C5-6205-4AE9-B261-171072854B1A}" name="Separation" dataDxfId="6" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{641DDC4E-2578-4498-8ED8-33F9AC71AB10}" name="Cohesion" dataDxfId="5" dataCellStyle="Input"/>
-    <tableColumn id="5" xr3:uid="{179A4AD1-A8EC-46AD-8FF9-141FCA114D6D}" name="Alignment" dataDxfId="4" dataCellStyle="Input"/>
-    <tableColumn id="6" xr3:uid="{151C99D6-CD01-4D17-8F3A-01FAB7A382A2}" name="Migration" dataDxfId="3" dataCellStyle="Input"/>
-    <tableColumn id="7" xr3:uid="{72FEDF7C-6E30-476A-A16F-D7F254AA231E}" name="Height Priority" dataCellStyle="Input"/>
-    <tableColumn id="8" xr3:uid="{CC5CE275-8057-44D1-8622-ADB69958C8BE}" name="Height Ignore" dataDxfId="2" dataCellStyle="Input"/>
-    <tableColumn id="9" xr3:uid="{8ADF89FF-9DC8-470A-997D-0B82F1446F55}" name="dt" dataDxfId="1" dataCellStyle="Input"/>
-    <tableColumn id="10" xr3:uid="{3688A395-01A4-4F8C-87AC-EBCEB8451D64}" name="Waggle Strength" dataDxfId="0" dataCellStyle="Input"/>
-    <tableColumn id="11" xr3:uid="{912B99C6-C266-42C5-BC8C-EACD040D1955}" name="Waggle Time" dataCellStyle="Input"/>
-    <tableColumn id="12" xr3:uid="{05614418-59D5-49AA-993F-A2600850294E}" name="# of Agents" dataCellStyle="Input"/>
-    <tableColumn id="13" xr3:uid="{C0646C68-4358-4ED2-A912-21AEA507E1B8}" name="Total Time" dataCellStyle="Input"/>
-    <tableColumn id="14" xr3:uid="{7CD3DE12-D699-4C70-BBAD-B2F8779BAD9B}" name="# of Thermals" dataCellStyle="Input"/>
-    <tableColumn id="15" xr3:uid="{48B0550F-2374-4EE4-803A-27DDC6FD82AB}" name="Neighbor Radius" dataCellStyle="Input"/>
-    <tableColumn id="17" xr3:uid="{C94C27D8-53C3-4038-A1D9-8F365CC794A2}" name="K" dataCellStyle="Input"/>
-    <tableColumn id="18" xr3:uid="{46F81300-083D-4FCE-823A-A3947F1ADB04}" name="FOV" dataCellStyle="Input"/>
-    <tableColumn id="19" xr3:uid="{CC929E8B-C7DA-44FB-921E-8105A3D9A803}" name="Surviving" dataCellStyle="Good"/>
-    <tableColumn id="20" xr3:uid="{4DF632DF-19A7-4CCB-95D0-9BDAB6140205}" name="Average Z of survivors" dataCellStyle="Good"/>
-    <tableColumn id="21" xr3:uid="{EDD2C0AE-273C-4242-A332-A79CB8E1C18B}" name="Flight Time" dataCellStyle="Good"/>
+    <tableColumn id="1" name="Date" xr3:uid="{517919BE-7171-41C2-BD81-2BD8FD4BA9AB}"/>
+    <tableColumn id="2" name="Time" xr3:uid="{32646A5F-2643-46B1-9978-5CED855C6BAA}"/>
+    <tableColumn id="3" name="Separation" dataDxfId="6" dataCellStyle="Input" xr3:uid="{C0D106C5-6205-4AE9-B261-171072854B1A}"/>
+    <tableColumn id="4" name="Cohesion" dataDxfId="5" dataCellStyle="Input" xr3:uid="{641DDC4E-2578-4498-8ED8-33F9AC71AB10}"/>
+    <tableColumn id="5" name="Alignment" dataDxfId="4" dataCellStyle="Input" xr3:uid="{179A4AD1-A8EC-46AD-8FF9-141FCA114D6D}"/>
+    <tableColumn id="6" name="Migration" dataDxfId="3" dataCellStyle="Input" xr3:uid="{151C99D6-CD01-4D17-8F3A-01FAB7A382A2}"/>
+    <tableColumn id="7" name="Height Priority" dataCellStyle="Input" xr3:uid="{72FEDF7C-6E30-476A-A16F-D7F254AA231E}"/>
+    <tableColumn id="8" name="Height Ignore" dataDxfId="2" dataCellStyle="Input" xr3:uid="{CC5CE275-8057-44D1-8622-ADB69958C8BE}"/>
+    <tableColumn id="9" name="dt" dataDxfId="1" dataCellStyle="Input" xr3:uid="{8ADF89FF-9DC8-470A-997D-0B82F1446F55}"/>
+    <tableColumn id="10" name="Waggle Strength" dataDxfId="0" dataCellStyle="Input" xr3:uid="{3688A395-01A4-4F8C-87AC-EBCEB8451D64}"/>
+    <tableColumn id="11" name="Waggle Time" dataCellStyle="Input" xr3:uid="{912B99C6-C266-42C5-BC8C-EACD040D1955}"/>
+    <tableColumn id="12" name="# of Agents" dataCellStyle="Input" xr3:uid="{05614418-59D5-49AA-993F-A2600850294E}"/>
+    <tableColumn id="13" name="Total Time" dataCellStyle="Input" xr3:uid="{C0646C68-4358-4ED2-A912-21AEA507E1B8}"/>
+    <tableColumn id="14" name="# of Thermals" dataCellStyle="Input" xr3:uid="{7CD3DE12-D699-4C70-BBAD-B2F8779BAD9B}"/>
+    <tableColumn id="15" name="Neighbor Radius" dataCellStyle="Input" xr3:uid="{48B0550F-2374-4EE4-803A-27DDC6FD82AB}"/>
+    <tableColumn id="17" name="K" dataCellStyle="Input" xr3:uid="{C94C27D8-53C3-4038-A1D9-8F365CC794A2}"/>
+    <tableColumn id="18" name="FOV" dataCellStyle="Input" xr3:uid="{46F81300-083D-4FCE-823A-A3947F1ADB04}"/>
+    <tableColumn id="19" name="Surviving" dataCellStyle="Good" xr3:uid="{CC929E8B-C7DA-44FB-921E-8105A3D9A803}"/>
+    <tableColumn id="20" name="Average Z of survivors" dataCellStyle="Good" xr3:uid="{4DF632DF-19A7-4CCB-95D0-9BDAB6140205}"/>
+    <tableColumn id="21" name="Flight Time" dataCellStyle="Good" xr3:uid="{EDD2C0AE-273C-4242-A332-A79CB8E1C18B}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
@@ -1284,34 +1328,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="5" width="5.77734375" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" customWidth="1"/>
-    <col min="12" max="12" width="8.21875" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
-    <col min="15" max="15" width="5.5546875" customWidth="1"/>
-    <col min="16" max="16" width="6.44140625" customWidth="1"/>
-    <col min="17" max="17" width="5.77734375" customWidth="1"/>
-    <col min="18" max="18" width="6.33203125" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" customWidth="1"/>
-    <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="4.6640625" customWidth="1"/>
-    <col min="22" max="22" width="7" customWidth="1"/>
-    <col min="23" max="23" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="true"/>
+    <col min="2" max="2" width="5" customWidth="true"/>
+    <col min="3" max="5" width="5.77734375" customWidth="true"/>
+    <col min="6" max="6" width="5.88671875" customWidth="true"/>
+    <col min="7" max="7" width="6.33203125" customWidth="true"/>
+    <col min="8" max="8" width="4.6640625" customWidth="true"/>
+    <col min="9" max="9" width="10.21875" customWidth="true"/>
+    <col min="10" max="10" width="6.21875" customWidth="true"/>
+    <col min="12" max="12" width="8.26953125" customWidth="true"/>
+    <col min="13" max="13" width="17.48828125" customWidth="true"/>
+    <col min="15" max="15" width="5.5546875" customWidth="true"/>
+    <col min="16" max="16" width="6.44140625" customWidth="true"/>
+    <col min="17" max="17" width="5.77734375" customWidth="true"/>
+    <col min="18" max="18" width="6.33203125" customWidth="true"/>
+    <col min="19" max="19" width="7.33203125" customWidth="true"/>
+    <col min="20" max="20" width="6" customWidth="true"/>
+    <col min="21" max="21" width="4.6640625" customWidth="true"/>
+    <col min="22" max="22" width="7" customWidth="true"/>
+    <col min="23" max="23" width="7.21875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1388,7 +1432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1396,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="D2" s="5">
         <v>-20</v>
@@ -1424,10 +1468,10 @@
         <v>40</v>
       </c>
       <c r="L2" s="3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="M2" s="3">
-        <v>2537.6384657643821</v>
+        <v>545.32945673477025</v>
       </c>
       <c r="O2">
         <v>7</v>
@@ -1466,7 +1510,7 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1521,7 +1565,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1576,7 +1620,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1634,7 +1678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1689,7 +1733,7 @@
         <v>106.4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1747,7 +1791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1802,7 +1846,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1860,7 +1904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1881,7 +1925,7 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1902,7 +1946,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1925,7 +1969,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1946,7 +1990,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1967,7 +2011,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1990,7 +2034,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2011,7 +2055,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -2030,7 +2074,7 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -2049,7 +2093,7 @@
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -2070,7 +2114,7 @@
         <v>936.5666135523162</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2089,7 +2133,7 @@
       </c>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -2108,7 +2152,7 @@
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -2127,7 +2171,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2146,7 +2190,7 @@
       </c>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -2167,7 +2211,7 @@
         <v>1480.0813924315723</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -2188,7 +2232,7 @@
         <v>1802.0267143636465</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2209,7 +2253,7 @@
         <v>805.97541697039958</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2228,7 +2272,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -2247,7 +2291,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -2268,7 +2312,7 @@
         <v>1335.1078219155152</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -2287,7 +2331,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2306,7 +2350,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -2327,7 +2371,7 @@
         <v>2502.1345715861339</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -2346,7 +2390,7 @@
       </c>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -2367,7 +2411,7 @@
         <v>1692.8703849181873</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -2388,7 +2432,7 @@
         <v>2572.4719309337597</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -2407,7 +2451,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -2426,7 +2470,7 @@
       </c>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2445,7 +2489,7 @@
       </c>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2464,7 +2508,7 @@
       </c>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2483,7 +2527,7 @@
       </c>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2502,7 +2546,7 @@
       </c>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2521,7 +2565,7 @@
       </c>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -2540,7 +2584,7 @@
       </c>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -2561,7 +2605,7 @@
         <v>315.75122511715415</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -2582,7 +2626,7 @@
         <v>179.5111996155043</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -2603,7 +2647,7 @@
         <v>680.89328368737654</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -2624,7 +2668,7 @@
         <v>60.444170583138309</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -2645,7 +2689,7 @@
         <v>306.46251611939141</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -2666,7 +2710,7 @@
         <v>1022.7226037491731</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2687,7 +2731,7 @@
         <v>524.21311430297283</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -2706,7 +2750,7 @@
       </c>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -2725,7 +2769,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -2744,7 +2788,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -2765,7 +2809,7 @@
         <v>385.26069063122509</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -2784,7 +2828,7 @@
       </c>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -2803,7 +2847,7 @@
       </c>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -2822,7 +2866,7 @@
       </c>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -2843,7 +2887,7 @@
         <v>409.11360749391292</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -2864,7 +2908,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -2885,7 +2929,7 @@
         <v>1594.0171603791832</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" x14ac:dyDescent="0.3">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -2921,11 +2965,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" customWidth="true"/>
+    <col min="9" max="9" width="11.6640625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2954,7 +2998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2983,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3012,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3041,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3070,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3099,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3128,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3157,7 +3201,7 @@
         <v>7.5884519722368706</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3186,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3215,7 +3259,7 @@
         <v>14.12841798433611</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3244,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3273,7 +3317,7 @@
         <v>57.493057852881904</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3302,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3331,7 +3375,7 @@
         <v>55.804506829739672</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3360,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3389,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3418,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3447,7 +3491,7 @@
         <v>67.672545269470248</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3476,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3505,7 +3549,7 @@
         <v>57.740155568967531</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3534,7 +3578,7 @@
         <v>22.643175158486237</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3563,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3592,7 +3636,7 @@
         <v>2.1369478109435907</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3621,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3650,7 +3694,7 @@
         <v>43.496043074433615</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3679,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3708,7 +3752,7 @@
         <v>32.032765825950221</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3737,7 +3781,7 @@
         <v>3.1622320797619392</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3766,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3795,7 +3839,7 @@
         <v>34.413155141176063</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3839,30 +3883,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="3.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="4.109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="2.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="3.109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="2.109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="2.109375" style="5" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="7.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" customWidth="true"/>
+    <col min="2" max="2" width="8.44140625" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="6.6640625" style="5" customWidth="true"/>
+    <col min="4" max="4" width="8.33203125" style="5" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="8.6640625" style="5" customWidth="true"/>
+    <col min="6" max="6" width="5.77734375" style="5" customWidth="true"/>
+    <col min="7" max="7" width="3.109375" style="5" customWidth="true"/>
+    <col min="8" max="8" width="4.109375" style="5" customWidth="true"/>
+    <col min="9" max="9" width="3.6640625" style="5" customWidth="true"/>
+    <col min="10" max="10" width="12.6640625" style="5" customWidth="true"/>
+    <col min="11" max="11" width="2.109375" style="5" customWidth="true"/>
+    <col min="12" max="12" width="3.109375" style="5" customWidth="true"/>
+    <col min="13" max="13" width="5.109375" style="5" customWidth="true"/>
+    <col min="14" max="14" width="2.109375" style="5" customWidth="true"/>
+    <col min="15" max="15" width="5.109375" style="5" customWidth="true"/>
+    <col min="16" max="16" width="11.6640625" style="5" customWidth="true"/>
+    <col min="17" max="17" width="2.109375" style="5" customWidth="true"/>
+    <col min="18" max="18" width="11.6640625" style="5" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="3.109375" style="2" customWidth="true"/>
+    <col min="20" max="20" width="11.6640625" style="2" customWidth="true"/>
+    <col min="21" max="21" width="7.6640625" style="2" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3927,7 +3971,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -3995,7 +4039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -4060,7 +4104,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4125,7 +4169,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -4190,7 +4234,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -4255,7 +4299,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -4320,7 +4364,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -4385,7 +4429,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -4450,7 +4494,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4515,7 +4559,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -4580,7 +4624,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -4645,7 +4689,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -4713,7 +4757,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -4778,7 +4822,7 @@
         <v>35027.99999999602</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -4840,7 +4884,7 @@
         <v>33599.399999997673</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -4905,7 +4949,7 @@
         <v>34393.39999999541</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4967,7 +5011,7 @@
         <v>34185.399999998022</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -5029,7 +5073,7 @@
         <v>44854.000000000749</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -5094,7 +5138,7 @@
         <v>41089.799999999734</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -5156,7 +5200,7 @@
         <v>33683.399999995439</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -5221,7 +5265,7 @@
         <v>38368.199999990931</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -5286,7 +5330,7 @@
         <v>29160.200000003344</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -5351,7 +5395,7 @@
         <v>26299.200000000703</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -5416,7 +5460,7 @@
         <v>35258.599999997146</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -5481,7 +5525,7 @@
         <v>38126.199999999233</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -5546,7 +5590,7 @@
         <v>41679.199999999524</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -5611,7 +5655,7 @@
         <v>37930.999999990832</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -5673,7 +5717,7 @@
         <v>42732.199999994467</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -5738,7 +5782,7 @@
         <v>40585.200000000761</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -5803,7 +5847,7 @@
         <v>34076.799999998162</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -5865,7 +5909,7 @@
         <v>36910.599999998631</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -5927,7 +5971,7 @@
         <v>38119.400000000707</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -5989,7 +6033,7 @@
         <v>36549.800000000418</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -6051,7 +6095,7 @@
         <v>33025.399999998008</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -6113,7 +6157,7 @@
         <v>35462.600000000064</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -6175,7 +6219,7 @@
         <v>31166.600000000191</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -6240,7 +6284,7 @@
         <v>36482.599999999664</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -6305,7 +6349,7 @@
         <v>50976.800000001349</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -6367,7 +6411,7 @@
         <v>36606.399999994253</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -6432,7 +6476,7 @@
         <v>39421.000000000116</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -6497,7 +6541,7 @@
         <v>33620.00000000446</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -6559,7 +6603,7 @@
         <v>30477.19999999983</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -6621,7 +6665,7 @@
         <v>34542.999999999862</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -6683,7 +6727,7 @@
         <v>40761.199999999873</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>63</v>
       </c>
@@ -6746,7 +6790,7 @@
         <v>37345.599999996375</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -6811,7 +6855,7 @@
         <v>33050.799999999683</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -6873,7 +6917,7 @@
         <v>35502.599999998631</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -6935,7 +6979,7 @@
         <v>39358.799999999595</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -6997,7 +7041,7 @@
         <v>30026.600000000013</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -7059,7 +7103,7 @@
         <v>33937.60000000037</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -7121,7 +7165,7 @@
         <v>27155.000000000033</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -7183,7 +7227,7 @@
         <v>30229.000000003762</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -7248,7 +7292,7 @@
         <v>48978.399999997098</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -7310,7 +7354,7 @@
         <v>30045.200000000623</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -7372,7 +7416,7 @@
         <v>28900.599999999948</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -7437,7 +7481,7 @@
         <v>38274.000000003412</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -7502,7 +7546,7 @@
         <v>36662.599999997838</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -7567,7 +7611,7 @@
         <v>38512.200000000266</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -7629,7 +7673,7 @@
         <v>29115.600000000741</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -7694,7 +7738,7 @@
         <v>37488.000000001339</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -7759,7 +7803,7 @@
         <v>38722.799999998148</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -7824,7 +7868,7 @@
         <v>28778.400000005924</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -7886,7 +7930,7 @@
         <v>27760.200000002103</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -7951,7 +7995,7 @@
         <v>26513.400000003559</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -8013,7 +8057,7 @@
         <v>32324.20000000286</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -8075,7 +8119,7 @@
         <v>22324.199999996672</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -8140,7 +8184,7 @@
         <v>33364.60000000638</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -8202,7 +8246,7 @@
         <v>30368.399999999674</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -8264,7 +8308,7 @@
         <v>32919.799999997398</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -8326,7 +8370,7 @@
         <v>32490.400000000889</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>63</v>
       </c>
@@ -8391,7 +8435,7 @@
         <v>32790.800000001815</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -8456,7 +8500,7 @@
         <v>32801.600000002523</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>63</v>
       </c>
@@ -8544,37 +8588,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78724697-14CA-4D59-A320-4AFE5FA0CB68}">
-  <dimension ref="A1:T74"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="P52" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12" style="5" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10.21875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="2.109375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.21875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="18.88671875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.48828125" customWidth="true"/>
+    <col min="2" max="2" width="8.26953125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="9.93359375" style="5" customWidth="true"/>
+    <col min="4" max="4" width="8.7109375" style="5" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="9.26953125" style="5" customWidth="true"/>
+    <col min="6" max="6" width="9.046875" style="5" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" style="5" customWidth="true"/>
+    <col min="8" max="8" width="12.046875" style="5" customWidth="true"/>
+    <col min="9" max="9" width="3.7109375" style="5" customWidth="true"/>
+    <col min="10" max="10" width="14.37890625" style="5" customWidth="true"/>
+    <col min="11" max="11" width="11.6015625" style="5" customWidth="true"/>
+    <col min="12" max="12" width="10.26953125" style="5" customWidth="true"/>
+    <col min="13" max="13" width="9.82421875" style="5" customWidth="true"/>
+    <col min="14" max="14" width="12.26953125" style="5" customWidth="true"/>
+    <col min="15" max="15" width="14.37890625" style="5" customWidth="true"/>
+    <col min="16" max="16" width="2.15625" style="5" customWidth="true"/>
+    <col min="17" max="17" width="11.7109375" style="5" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="8.26953125" style="2" customWidth="true"/>
+    <col min="19" max="19" width="18.93359375" style="2" customWidth="true"/>
+    <col min="20" max="20" width="9.93359375" style="2" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -8636,7 +8680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -8698,7 +8742,7 @@
         <v>29165.200000000514</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -8760,7 +8804,7 @@
         <v>32148.999999999323</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -8819,7 +8863,7 @@
         <v>28879.999999998843</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -8881,7 +8925,7 @@
         <v>29092.200000003271</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -8943,7 +8987,7 @@
         <v>29527.200000003089</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -9002,7 +9046,7 @@
         <v>26128.399999999743</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -9061,7 +9105,7 @@
         <v>36629.599999998638</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -9120,7 +9164,7 @@
         <v>29255.599999999486</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -9179,7 +9223,7 @@
         <v>32351.600000000621</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>119</v>
       </c>
@@ -9238,7 +9282,7 @@
         <v>37064.200000000121</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -9300,7 +9344,7 @@
         <v>35225.799999999879</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -9359,7 +9403,7 @@
         <v>32775.199999999699</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -9418,7 +9462,7 @@
         <v>42064.800000000119</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -9480,7 +9524,7 @@
         <v>42737.199999997887</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -9539,7 +9583,7 @@
         <v>43286.000000000298</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -9598,7 +9642,7 @@
         <v>48894.000000000153</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -9657,7 +9701,7 @@
         <v>39808.199999997771</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -9719,7 +9763,7 @@
         <v>43696.200000005461</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -9778,7 +9822,7 @@
         <v>33738.5999999954</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -9837,7 +9881,7 @@
         <v>39497.599999998303</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -9896,7 +9940,7 @@
         <v>30571.80000000216</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>119</v>
       </c>
@@ -9955,7 +9999,7 @@
         <v>40042.999999999811</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -10017,7 +10061,7 @@
         <v>37158.200000003693</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -10079,7 +10123,7 @@
         <v>43576.199999995697</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -10141,7 +10185,7 @@
         <v>55667.40000000225</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -10200,7 +10244,7 @@
         <v>34088.600000001556</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -10259,7 +10303,7 @@
         <v>34135.199999999757</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -10321,7 +10365,7 @@
         <v>38286.199999988166</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -10380,7 +10424,7 @@
         <v>30056.200000001008</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -10439,7 +10483,7 @@
         <v>38416.799999997143</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -10501,7 +10545,7 @@
         <v>50684.199999990728</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -10560,7 +10604,7 @@
         <v>40810.600000001854</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -10622,7 +10666,7 @@
         <v>49346.599999989463</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>119</v>
       </c>
@@ -10684,7 +10728,7 @@
         <v>43390.600000006285</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -10743,7 +10787,7 @@
         <v>30349.800000000203</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -10802,7 +10846,7 @@
         <v>39633.200000000492</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -10861,7 +10905,7 @@
         <v>30935.800000001906</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -10920,7 +10964,7 @@
         <v>27782.60000000049</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -10979,7 +11023,7 @@
         <v>28711.399999999983</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -11038,7 +11082,7 @@
         <v>32224.199999999935</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -11097,7 +11141,7 @@
         <v>24482.600000002334</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -11156,7 +11200,7 @@
         <v>21468.800000000483</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>119</v>
       </c>
@@ -11218,7 +11262,7 @@
         <v>39340.599999995233</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>119</v>
       </c>
@@ -11280,7 +11324,7 @@
         <v>38564.999999998588</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -11342,7 +11386,7 @@
         <v>40955.599999999824</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -11404,7 +11448,7 @@
         <v>33751.199999989847</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -11466,7 +11510,7 @@
         <v>38959.999999998297</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -11528,7 +11572,7 @@
         <v>37768.400000006339</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -11590,7 +11634,7 @@
         <v>31820.400000003734</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -11649,7 +11693,7 @@
         <v>30756.000000000269</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -11708,7 +11752,7 @@
         <v>28571.800000001876</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>119</v>
       </c>
@@ -11767,7 +11811,7 @@
         <v>30477.199999999561</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -11829,7 +11873,7 @@
         <v>31562.200000002707</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -11888,7 +11932,7 @@
         <v>18789.4000000009</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -11947,7 +11991,7 @@
         <v>34111.80000000068</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -12006,7 +12050,7 @@
         <v>31760.200000002791</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -12068,7 +12112,7 @@
         <v>32771.400000002293</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -12130,7 +12174,7 @@
         <v>32932.400000005939</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -12192,7 +12236,7 @@
         <v>33675.199999998025</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -12254,7 +12298,7 @@
         <v>30980.800000003019</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -12313,7 +12357,7 @@
         <v>30653.400000000209</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>179</v>
       </c>
@@ -12372,7 +12416,7 @@
         <v>30942.000000001513</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>179</v>
       </c>
@@ -12431,7 +12475,7 @@
         <v>31707.200000002853</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>179</v>
       </c>
@@ -12490,7 +12534,7 @@
         <v>31359.600000003156</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>179</v>
       </c>
@@ -12549,7 +12593,7 @@
         <v>31477.600000001203</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -12608,7 +12652,7 @@
         <v>31041.999999999549</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>186</v>
       </c>
@@ -12667,7 +12711,7 @@
         <v>33213.999999996209</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>188</v>
       </c>
@@ -12729,7 +12773,7 @@
         <v>43995.00000000008</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -12791,7 +12835,7 @@
         <v>38667.599999999715</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>192</v>
       </c>
@@ -12850,7 +12894,7 @@
         <v>29930.399999998794</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>194</v>
       </c>
@@ -12909,7 +12953,7 @@
         <v>28990.999999999593</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>196</v>
       </c>
@@ -12969,7 +13013,7 @@
         <v>32166.199999998353</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -13029,6 +13073,437 @@
       </c>
       <c r="T74" s="2">
         <v>43606.599999992613</v>
+      </c>
+    </row>
+    <row r="75" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E75" s="5">
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="F75" s="5">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G75" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H75" s="5">
+        <v>200</v>
+      </c>
+      <c r="I75" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="J75" s="5">
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="K75" s="5">
+        <v>24</v>
+      </c>
+      <c r="L75" s="5">
+        <v>40</v>
+      </c>
+      <c r="M75" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N75" s="5">
+        <v>6</v>
+      </c>
+      <c r="O75" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P75" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q75" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R75" s="2">
+        <v>3</v>
+      </c>
+      <c r="S75" s="2">
+        <v>487.79800055949431</v>
+      </c>
+      <c r="T75" s="2">
+        <v>42264.000000003056</v>
+      </c>
+    </row>
+    <row r="76" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>202</v>
+      </c>
+      <c r="B76" t="s">
+        <v>203</v>
+      </c>
+      <c r="C76" s="5">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E76" s="5">
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="F76" s="5">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G76" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H76" s="5">
+        <v>200</v>
+      </c>
+      <c r="I76" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="J76" s="5">
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="K76" s="5">
+        <v>24</v>
+      </c>
+      <c r="L76" s="5">
+        <v>40</v>
+      </c>
+      <c r="M76" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N76" s="5">
+        <v>6</v>
+      </c>
+      <c r="O76" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P76" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q76" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R76" s="2">
+        <v>2</v>
+      </c>
+      <c r="S76" s="2">
+        <v>379.26521868741338</v>
+      </c>
+      <c r="T76" s="2">
+        <v>48968.799999999152</v>
+      </c>
+    </row>
+    <row r="77" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>204</v>
+      </c>
+      <c r="B77" t="s">
+        <v>205</v>
+      </c>
+      <c r="C77" s="5">
+        <v>1</v>
+      </c>
+      <c r="D77" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E77" s="5">
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="F77" s="5">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G77" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H77" s="5">
+        <v>200</v>
+      </c>
+      <c r="I77" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="J77" s="5">
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="K77" s="5">
+        <v>24</v>
+      </c>
+      <c r="L77" s="5">
+        <v>10</v>
+      </c>
+      <c r="M77" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N77" s="5">
+        <v>6</v>
+      </c>
+      <c r="O77" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P77" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q77" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R77" s="2">
+        <v>0</v>
+      </c>
+      <c r="T77" s="2">
+        <v>9361.2000000002954</v>
+      </c>
+    </row>
+    <row r="78" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78" t="s">
+        <v>207</v>
+      </c>
+      <c r="C78" s="5">
+        <v>1</v>
+      </c>
+      <c r="D78" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E78" s="5">
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="F78" s="5">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G78" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H78" s="5">
+        <v>200</v>
+      </c>
+      <c r="I78" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="J78" s="5">
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="K78" s="5">
+        <v>24</v>
+      </c>
+      <c r="L78" s="5">
+        <v>10</v>
+      </c>
+      <c r="M78" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N78" s="5">
+        <v>6</v>
+      </c>
+      <c r="O78" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P78" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q78" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R78" s="2">
+        <v>2</v>
+      </c>
+      <c r="S78" s="2">
+        <v>689.86269399814921</v>
+      </c>
+      <c r="T78" s="2">
+        <v>10982.799999997991</v>
+      </c>
+    </row>
+    <row r="79" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>208</v>
+      </c>
+      <c r="B79" t="s">
+        <v>209</v>
+      </c>
+      <c r="C79" s="5">
+        <v>1</v>
+      </c>
+      <c r="D79" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E79" s="5">
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="F79" s="5">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G79" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H79" s="5">
+        <v>200</v>
+      </c>
+      <c r="I79" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="J79" s="5">
+        <v>5.2359877559829883E-2</v>
+      </c>
+      <c r="K79" s="5">
+        <v>24</v>
+      </c>
+      <c r="L79" s="5">
+        <v>10</v>
+      </c>
+      <c r="M79" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N79" s="5">
+        <v>6</v>
+      </c>
+      <c r="O79" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P79" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q79" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R79" s="2">
+        <v>1</v>
+      </c>
+      <c r="S79" s="2">
+        <v>248.01266028120637</v>
+      </c>
+      <c r="T79" s="2">
+        <v>8193.999999999407</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C80" s="5">
+        <v>1</v>
+      </c>
+      <c r="D80" s="5">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="E80" s="5">
+        <v>1.0000000000000001e-20</v>
+      </c>
+      <c r="F80" s="5">
+        <v>1.0000000000000001e-21</v>
+      </c>
+      <c r="G80" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H80" s="5">
+        <v>200</v>
+      </c>
+      <c r="I80" s="5">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="J80" s="5">
+        <v>0.052359877559829883</v>
+      </c>
+      <c r="K80" s="5">
+        <v>24</v>
+      </c>
+      <c r="L80" s="5">
+        <v>40</v>
+      </c>
+      <c r="M80" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N80" s="5">
+        <v>6</v>
+      </c>
+      <c r="O80" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P80" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q80" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R80" s="2">
+        <v>2</v>
+      </c>
+      <c r="S80" s="2">
+        <v>1473.6720555650209</v>
+      </c>
+      <c r="T80" s="2">
+        <v>51456.400000001871</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C81" s="5">
+        <v>1</v>
+      </c>
+      <c r="D81" s="5">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="E81" s="5">
+        <v>1.0000000000000001e-20</v>
+      </c>
+      <c r="F81" s="5">
+        <v>1.0000000000000001e-21</v>
+      </c>
+      <c r="G81" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H81" s="5">
+        <v>200</v>
+      </c>
+      <c r="I81" s="5">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="J81" s="5">
+        <v>0.052359877559829883</v>
+      </c>
+      <c r="K81" s="5">
+        <v>24</v>
+      </c>
+      <c r="L81" s="5">
+        <v>40</v>
+      </c>
+      <c r="M81" s="5">
+        <v>1800</v>
+      </c>
+      <c r="N81" s="5">
+        <v>6</v>
+      </c>
+      <c r="O81" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P81" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q81" s="5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R81" s="2">
+        <v>4</v>
+      </c>
+      <c r="S81" s="2">
+        <v>545.32945673477025</v>
+      </c>
+      <c r="T81" s="2">
+        <v>45408.199999999881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conflict Avoidance Part 2: Agent + Swarm
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD705FE-2363-44BE-A536-1712D249D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7324AAD-1900-4040-8301-F5DB37B1FC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input (First Sheet Always)" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Log 06-28" sheetId="3" r:id="rId3"/>
     <sheet name="Log 06-29" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -751,18 +751,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038484"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038484"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -822,37 +822,35 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="true"/>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="true"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="true"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="true"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="true"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -864,7 +862,7 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -874,14 +872,14 @@
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -889,7 +887,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="false">
+      <border outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -897,21 +895,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="false">
+      <border outline="0">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -921,14 +919,14 @@
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -936,7 +934,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="false">
+      <border outline="0">
         <left style="thin">
           <color rgb="FF7F7F7F"/>
         </left>
@@ -944,14 +942,14 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <border outline="false">
+      <border outline="0">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <border outline="false">
+      <border outline="0">
         <right style="thin">
           <color rgb="FF7F7F7F"/>
         </right>
@@ -971,61 +969,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="1" name="Table1" displayName="Table1" ref="A1:U73" totalsRowShown="false" headerRowCellStyle="Good" dataCellStyle="Good" mc:Ignorable="xr xr3" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}" name="Table1" displayName="Table1" ref="A1:U73" totalsRowShown="0" headerRowCellStyle="Good" dataCellStyle="Good">
   <autoFilter ref="A1:U73" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}"/>
   <tableColumns count="21">
-    <tableColumn id="1" name="Date" xr3:uid="{CD2AE5F0-A067-48DC-945F-0570E6312B06}"/>
-    <tableColumn id="2" name="Time" xr3:uid="{124F9F36-5D64-42C9-B806-47D006C6CA9A}"/>
-    <tableColumn id="3" name="Separation" dataDxfId="13" dataCellStyle="Input" xr3:uid="{D7BF650C-D78F-47FF-A191-5F7C2A908175}"/>
-    <tableColumn id="4" name="Cohesion" dataDxfId="12" dataCellStyle="Input" xr3:uid="{63B5EB73-2B29-4135-ADE4-880D10883200}"/>
-    <tableColumn id="5" name="Alignment" dataDxfId="11" dataCellStyle="Input" xr3:uid="{B9124B5C-D0AE-4010-BC14-B88C64B9756E}"/>
-    <tableColumn id="6" name="Migration" dataDxfId="10" dataCellStyle="Input" xr3:uid="{BFB8E62F-AE8F-403E-92F6-61D4A7E19ADA}"/>
-    <tableColumn id="7" name="Height Priority" dataCellStyle="Input" xr3:uid="{2936402B-09B3-4C5D-B402-9D28E0F2E8A8}"/>
-    <tableColumn id="8" name="Height Ignore" dataDxfId="9" dataCellStyle="Input" xr3:uid="{E7AEB934-FAB1-4B69-BE53-62A8F39A764C}"/>
-    <tableColumn id="9" name="dt" dataDxfId="8" dataCellStyle="Input" xr3:uid="{736093B2-EF64-4847-B7C4-2E9CDB164008}"/>
-    <tableColumn id="10" name="Waggle Strength" dataDxfId="7" dataCellStyle="Input" xr3:uid="{C5795275-E854-4EFB-88B9-C49B37FF6999}"/>
-    <tableColumn id="11" name="Waggle Time" dataCellStyle="Input" xr3:uid="{A6DEE2DA-660A-4D68-987E-58E933151945}"/>
-    <tableColumn id="12" name="# of Agents" dataCellStyle="Input" xr3:uid="{9FDB18DD-6007-41EC-9734-C49EC48B769A}"/>
-    <tableColumn id="13" name="Total Time" dataCellStyle="Input" xr3:uid="{C6C801F0-B377-4F31-A463-104D29538A52}"/>
-    <tableColumn id="14" name="# of Thermals" dataCellStyle="Input" xr3:uid="{F01BD334-4E3B-408C-AA8F-9A18BE4AA0BD}"/>
-    <tableColumn id="15" name="Neighbor Radius" dataCellStyle="Input" xr3:uid="{2D9CAFF3-8B5B-409E-8F68-FBCE1BBB76DF}"/>
-    <tableColumn id="16" name="Neighbor Angle Range" dataCellStyle="Input" xr3:uid="{E107D01D-AB0E-4655-9B1A-B57B0C63EC40}"/>
-    <tableColumn id="17" name="K" dataCellStyle="Input" xr3:uid="{91A8CDD3-26BE-4A07-A1A4-F64FB8CB0B40}"/>
-    <tableColumn id="18" name="FOV" dataCellStyle="Input" xr3:uid="{65DCF8D9-31A5-4CC2-87E2-88950F9548CF}"/>
-    <tableColumn id="19" name="Surviving" dataCellStyle="Good" xr3:uid="{403513BC-6E74-4FB8-BBA8-258B934381A5}"/>
-    <tableColumn id="20" name="Average Z of survivors" dataCellStyle="Good" xr3:uid="{9C3C23D8-78A8-4FC2-B90D-4AAEA40043BA}"/>
-    <tableColumn id="21" name="Flight Time" dataCellStyle="Good" xr3:uid="{D2031C1F-0DC7-4809-88C0-819C871DDDA0}"/>
+    <tableColumn id="1" xr3:uid="{CD2AE5F0-A067-48DC-945F-0570E6312B06}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{124F9F36-5D64-42C9-B806-47D006C6CA9A}" name="Time"/>
+    <tableColumn id="3" xr3:uid="{D7BF650C-D78F-47FF-A191-5F7C2A908175}" name="Separation" dataDxfId="13" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{63B5EB73-2B29-4135-ADE4-880D10883200}" name="Cohesion" dataDxfId="12" dataCellStyle="Input"/>
+    <tableColumn id="5" xr3:uid="{B9124B5C-D0AE-4010-BC14-B88C64B9756E}" name="Alignment" dataDxfId="11" dataCellStyle="Input"/>
+    <tableColumn id="6" xr3:uid="{BFB8E62F-AE8F-403E-92F6-61D4A7E19ADA}" name="Migration" dataDxfId="10" dataCellStyle="Input"/>
+    <tableColumn id="7" xr3:uid="{2936402B-09B3-4C5D-B402-9D28E0F2E8A8}" name="Height Priority" dataCellStyle="Input"/>
+    <tableColumn id="8" xr3:uid="{E7AEB934-FAB1-4B69-BE53-62A8F39A764C}" name="Height Ignore" dataDxfId="9" dataCellStyle="Input"/>
+    <tableColumn id="9" xr3:uid="{736093B2-EF64-4847-B7C4-2E9CDB164008}" name="dt" dataDxfId="8" dataCellStyle="Input"/>
+    <tableColumn id="10" xr3:uid="{C5795275-E854-4EFB-88B9-C49B37FF6999}" name="Waggle Strength" dataDxfId="7" dataCellStyle="Input"/>
+    <tableColumn id="11" xr3:uid="{A6DEE2DA-660A-4D68-987E-58E933151945}" name="Waggle Time" dataCellStyle="Input"/>
+    <tableColumn id="12" xr3:uid="{9FDB18DD-6007-41EC-9734-C49EC48B769A}" name="# of Agents" dataCellStyle="Input"/>
+    <tableColumn id="13" xr3:uid="{C6C801F0-B377-4F31-A463-104D29538A52}" name="Total Time" dataCellStyle="Input"/>
+    <tableColumn id="14" xr3:uid="{F01BD334-4E3B-408C-AA8F-9A18BE4AA0BD}" name="# of Thermals" dataCellStyle="Input"/>
+    <tableColumn id="15" xr3:uid="{2D9CAFF3-8B5B-409E-8F68-FBCE1BBB76DF}" name="Neighbor Radius" dataCellStyle="Input"/>
+    <tableColumn id="16" xr3:uid="{E107D01D-AB0E-4655-9B1A-B57B0C63EC40}" name="Neighbor Angle Range" dataCellStyle="Input"/>
+    <tableColumn id="17" xr3:uid="{91A8CDD3-26BE-4A07-A1A4-F64FB8CB0B40}" name="K" dataCellStyle="Input"/>
+    <tableColumn id="18" xr3:uid="{65DCF8D9-31A5-4CC2-87E2-88950F9548CF}" name="FOV" dataCellStyle="Input"/>
+    <tableColumn id="19" xr3:uid="{403513BC-6E74-4FB8-BBA8-258B934381A5}" name="Surviving" dataCellStyle="Good"/>
+    <tableColumn id="20" xr3:uid="{9C3C23D8-78A8-4FC2-B90D-4AAEA40043BA}" name="Average Z of survivors" dataCellStyle="Good"/>
+    <tableColumn id="21" xr3:uid="{D2031C1F-0DC7-4809-88C0-819C871DDDA0}" name="Flight Time" dataCellStyle="Good"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="2" name="Table13" displayName="Table13" ref="A1:T73" totalsRowShown="false" headerRowCellStyle="Good" dataCellStyle="Good" mc:Ignorable="xr xr3" xr:uid="{C51EEC99-3A6C-45AC-AAA7-E48D93D343CE}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C51EEC99-3A6C-45AC-AAA7-E48D93D343CE}" name="Table13" displayName="Table13" ref="A1:T73" totalsRowShown="0" headerRowCellStyle="Good" dataCellStyle="Good">
   <autoFilter ref="A1:T73" xr:uid="{6DA8C114-7B87-40FD-9227-C941B66417C2}"/>
   <tableColumns count="20">
-    <tableColumn id="1" name="Date" xr3:uid="{517919BE-7171-41C2-BD81-2BD8FD4BA9AB}"/>
-    <tableColumn id="2" name="Time" xr3:uid="{32646A5F-2643-46B1-9978-5CED855C6BAA}"/>
-    <tableColumn id="3" name="Separation" dataDxfId="6" dataCellStyle="Input" xr3:uid="{C0D106C5-6205-4AE9-B261-171072854B1A}"/>
-    <tableColumn id="4" name="Cohesion" dataDxfId="5" dataCellStyle="Input" xr3:uid="{641DDC4E-2578-4498-8ED8-33F9AC71AB10}"/>
-    <tableColumn id="5" name="Alignment" dataDxfId="4" dataCellStyle="Input" xr3:uid="{179A4AD1-A8EC-46AD-8FF9-141FCA114D6D}"/>
-    <tableColumn id="6" name="Migration" dataDxfId="3" dataCellStyle="Input" xr3:uid="{151C99D6-CD01-4D17-8F3A-01FAB7A382A2}"/>
-    <tableColumn id="7" name="Height Priority" dataCellStyle="Input" xr3:uid="{72FEDF7C-6E30-476A-A16F-D7F254AA231E}"/>
-    <tableColumn id="8" name="Height Ignore" dataDxfId="2" dataCellStyle="Input" xr3:uid="{CC5CE275-8057-44D1-8622-ADB69958C8BE}"/>
-    <tableColumn id="9" name="dt" dataDxfId="1" dataCellStyle="Input" xr3:uid="{8ADF89FF-9DC8-470A-997D-0B82F1446F55}"/>
-    <tableColumn id="10" name="Waggle Strength" dataDxfId="0" dataCellStyle="Input" xr3:uid="{3688A395-01A4-4F8C-87AC-EBCEB8451D64}"/>
-    <tableColumn id="11" name="Waggle Time" dataCellStyle="Input" xr3:uid="{912B99C6-C266-42C5-BC8C-EACD040D1955}"/>
-    <tableColumn id="12" name="# of Agents" dataCellStyle="Input" xr3:uid="{05614418-59D5-49AA-993F-A2600850294E}"/>
-    <tableColumn id="13" name="Total Time" dataCellStyle="Input" xr3:uid="{C0646C68-4358-4ED2-A912-21AEA507E1B8}"/>
-    <tableColumn id="14" name="# of Thermals" dataCellStyle="Input" xr3:uid="{7CD3DE12-D699-4C70-BBAD-B2F8779BAD9B}"/>
-    <tableColumn id="15" name="Neighbor Radius" dataCellStyle="Input" xr3:uid="{48B0550F-2374-4EE4-803A-27DDC6FD82AB}"/>
-    <tableColumn id="17" name="K" dataCellStyle="Input" xr3:uid="{C94C27D8-53C3-4038-A1D9-8F365CC794A2}"/>
-    <tableColumn id="18" name="FOV" dataCellStyle="Input" xr3:uid="{46F81300-083D-4FCE-823A-A3947F1ADB04}"/>
-    <tableColumn id="19" name="Surviving" dataCellStyle="Good" xr3:uid="{CC929E8B-C7DA-44FB-921E-8105A3D9A803}"/>
-    <tableColumn id="20" name="Average Z of survivors" dataCellStyle="Good" xr3:uid="{4DF632DF-19A7-4CCB-95D0-9BDAB6140205}"/>
-    <tableColumn id="21" name="Flight Time" dataCellStyle="Good" xr3:uid="{EDD2C0AE-273C-4242-A332-A79CB8E1C18B}"/>
+    <tableColumn id="1" xr3:uid="{517919BE-7171-41C2-BD81-2BD8FD4BA9AB}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{32646A5F-2643-46B1-9978-5CED855C6BAA}" name="Time"/>
+    <tableColumn id="3" xr3:uid="{C0D106C5-6205-4AE9-B261-171072854B1A}" name="Separation" dataDxfId="6" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{641DDC4E-2578-4498-8ED8-33F9AC71AB10}" name="Cohesion" dataDxfId="5" dataCellStyle="Input"/>
+    <tableColumn id="5" xr3:uid="{179A4AD1-A8EC-46AD-8FF9-141FCA114D6D}" name="Alignment" dataDxfId="4" dataCellStyle="Input"/>
+    <tableColumn id="6" xr3:uid="{151C99D6-CD01-4D17-8F3A-01FAB7A382A2}" name="Migration" dataDxfId="3" dataCellStyle="Input"/>
+    <tableColumn id="7" xr3:uid="{72FEDF7C-6E30-476A-A16F-D7F254AA231E}" name="Height Priority" dataCellStyle="Input"/>
+    <tableColumn id="8" xr3:uid="{CC5CE275-8057-44D1-8622-ADB69958C8BE}" name="Height Ignore" dataDxfId="2" dataCellStyle="Input"/>
+    <tableColumn id="9" xr3:uid="{8ADF89FF-9DC8-470A-997D-0B82F1446F55}" name="dt" dataDxfId="1" dataCellStyle="Input"/>
+    <tableColumn id="10" xr3:uid="{3688A395-01A4-4F8C-87AC-EBCEB8451D64}" name="Waggle Strength" dataDxfId="0" dataCellStyle="Input"/>
+    <tableColumn id="11" xr3:uid="{912B99C6-C266-42C5-BC8C-EACD040D1955}" name="Waggle Time" dataCellStyle="Input"/>
+    <tableColumn id="12" xr3:uid="{05614418-59D5-49AA-993F-A2600850294E}" name="# of Agents" dataCellStyle="Input"/>
+    <tableColumn id="13" xr3:uid="{C0646C68-4358-4ED2-A912-21AEA507E1B8}" name="Total Time" dataCellStyle="Input"/>
+    <tableColumn id="14" xr3:uid="{7CD3DE12-D699-4C70-BBAD-B2F8779BAD9B}" name="# of Thermals" dataCellStyle="Input"/>
+    <tableColumn id="15" xr3:uid="{48B0550F-2374-4EE4-803A-27DDC6FD82AB}" name="Neighbor Radius" dataCellStyle="Input"/>
+    <tableColumn id="17" xr3:uid="{C94C27D8-53C3-4038-A1D9-8F365CC794A2}" name="K" dataCellStyle="Input"/>
+    <tableColumn id="18" xr3:uid="{46F81300-083D-4FCE-823A-A3947F1ADB04}" name="FOV" dataCellStyle="Input"/>
+    <tableColumn id="19" xr3:uid="{CC929E8B-C7DA-44FB-921E-8105A3D9A803}" name="Surviving" dataCellStyle="Good"/>
+    <tableColumn id="20" xr3:uid="{4DF632DF-19A7-4CCB-95D0-9BDAB6140205}" name="Average Z of survivors" dataCellStyle="Good"/>
+    <tableColumn id="21" xr3:uid="{EDD2C0AE-273C-4242-A332-A79CB8E1C18B}" name="Flight Time" dataCellStyle="Good"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1328,34 +1326,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="true"/>
-    <col min="2" max="2" width="5" customWidth="true"/>
-    <col min="3" max="5" width="5.77734375" customWidth="true"/>
-    <col min="6" max="6" width="5.88671875" customWidth="true"/>
-    <col min="7" max="7" width="6.33203125" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.21875" customWidth="true"/>
-    <col min="10" max="10" width="6.21875" customWidth="true"/>
-    <col min="12" max="12" width="8.26953125" customWidth="true"/>
-    <col min="13" max="13" width="17.48828125" customWidth="true"/>
-    <col min="15" max="15" width="5.5546875" customWidth="true"/>
-    <col min="16" max="16" width="6.44140625" customWidth="true"/>
-    <col min="17" max="17" width="5.77734375" customWidth="true"/>
-    <col min="18" max="18" width="6.33203125" customWidth="true"/>
-    <col min="19" max="19" width="7.33203125" customWidth="true"/>
-    <col min="20" max="20" width="6" customWidth="true"/>
-    <col min="21" max="21" width="4.6640625" customWidth="true"/>
-    <col min="22" max="22" width="7" customWidth="true"/>
-    <col min="23" max="23" width="7.21875" customWidth="true"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="5" width="5.77734375" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="6.21875" customWidth="1"/>
+    <col min="12" max="12" width="8.21875" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" customWidth="1"/>
+    <col min="16" max="16" width="6.44140625" customWidth="1"/>
+    <col min="17" max="17" width="5.77734375" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" customWidth="1"/>
+    <col min="20" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" customWidth="1"/>
+    <col min="22" max="22" width="7" customWidth="1"/>
+    <col min="23" max="23" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1432,7 +1430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>-6</v>
       </c>
       <c r="D2" s="5">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>-21</v>
@@ -1458,14 +1456,13 @@
         <v>0.2</v>
       </c>
       <c r="I2" s="5">
-        <f>PI()/60</f>
-        <v>5.2359877559829883E-2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="5">
         <v>24</v>
       </c>
       <c r="K2" s="5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L2" s="3">
         <v>4</v>
@@ -1510,7 +1507,7 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1565,7 +1562,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1620,7 +1617,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1678,7 +1675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1733,7 +1730,7 @@
         <v>106.4</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1791,7 +1788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1846,7 +1843,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1904,7 +1901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1925,7 +1922,7 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1946,7 +1943,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1969,7 +1966,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1990,7 +1987,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2011,7 +2008,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -2034,7 +2031,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2055,7 +2052,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -2074,7 +2071,7 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -2093,7 +2090,7 @@
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -2114,7 +2111,7 @@
         <v>936.5666135523162</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2133,7 +2130,7 @@
       </c>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -2152,7 +2149,7 @@
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -2171,7 +2168,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2190,7 +2187,7 @@
       </c>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -2211,7 +2208,7 @@
         <v>1480.0813924315723</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -2232,7 +2229,7 @@
         <v>1802.0267143636465</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>805.97541697039958</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2272,7 +2269,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -2291,7 +2288,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -2312,7 +2309,7 @@
         <v>1335.1078219155152</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -2331,7 +2328,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2350,7 +2347,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -2371,7 +2368,7 @@
         <v>2502.1345715861339</v>
       </c>
     </row>
-    <row r="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -2390,7 +2387,7 @@
       </c>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -2411,7 +2408,7 @@
         <v>1692.8703849181873</v>
       </c>
     </row>
-    <row r="35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -2432,7 +2429,7 @@
         <v>2572.4719309337597</v>
       </c>
     </row>
-    <row r="36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -2451,7 +2448,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -2470,7 +2467,7 @@
       </c>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2489,7 +2486,7 @@
       </c>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2508,7 +2505,7 @@
       </c>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2527,7 +2524,7 @@
       </c>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2546,7 +2543,7 @@
       </c>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2565,7 +2562,7 @@
       </c>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -2584,7 +2581,7 @@
       </c>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -2605,7 +2602,7 @@
         <v>315.75122511715415</v>
       </c>
     </row>
-    <row r="45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -2626,7 +2623,7 @@
         <v>179.5111996155043</v>
       </c>
     </row>
-    <row r="46" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -2647,7 +2644,7 @@
         <v>680.89328368737654</v>
       </c>
     </row>
-    <row r="47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -2668,7 +2665,7 @@
         <v>60.444170583138309</v>
       </c>
     </row>
-    <row r="48" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -2689,7 +2686,7 @@
         <v>306.46251611939141</v>
       </c>
     </row>
-    <row r="49" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -2710,7 +2707,7 @@
         <v>1022.7226037491731</v>
       </c>
     </row>
-    <row r="50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2731,7 +2728,7 @@
         <v>524.21311430297283</v>
       </c>
     </row>
-    <row r="51" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -2750,7 +2747,7 @@
       </c>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -2769,7 +2766,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -2788,7 +2785,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -2809,7 +2806,7 @@
         <v>385.26069063122509</v>
       </c>
     </row>
-    <row r="55" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -2828,7 +2825,7 @@
       </c>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -2847,7 +2844,7 @@
       </c>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -2866,7 +2863,7 @@
       </c>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -2887,7 +2884,7 @@
         <v>409.11360749391292</v>
       </c>
     </row>
-    <row r="59" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="60" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -2929,7 +2926,7 @@
         <v>1594.0171603791832</v>
       </c>
     </row>
-    <row r="61" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -2965,11 +2962,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="8.77734375" customWidth="true"/>
-    <col min="9" max="9" width="11.6640625" customWidth="true"/>
+    <col min="8" max="8" width="8.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2998,7 +2995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3027,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3056,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3085,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3114,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3143,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3172,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3201,7 +3198,7 @@
         <v>7.5884519722368706</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3230,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3259,7 +3256,7 @@
         <v>14.12841798433611</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3288,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3317,7 +3314,7 @@
         <v>57.493057852881904</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3346,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3375,7 +3372,7 @@
         <v>55.804506829739672</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3404,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3433,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3462,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3491,7 +3488,7 @@
         <v>67.672545269470248</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3520,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3549,7 +3546,7 @@
         <v>57.740155568967531</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3578,7 +3575,7 @@
         <v>22.643175158486237</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3607,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3636,7 +3633,7 @@
         <v>2.1369478109435907</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3694,7 +3691,7 @@
         <v>43.496043074433615</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3723,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3752,7 +3749,7 @@
         <v>32.032765825950221</v>
       </c>
     </row>
-    <row r="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3781,7 +3778,7 @@
         <v>3.1622320797619392</v>
       </c>
     </row>
-    <row r="29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3810,7 +3807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3839,7 +3836,7 @@
         <v>34.413155141176063</v>
       </c>
     </row>
-    <row r="31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3883,30 +3880,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="true"/>
-    <col min="2" max="2" width="8.44140625" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="6.6640625" style="5" customWidth="true"/>
-    <col min="4" max="4" width="8.33203125" style="5" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="8.6640625" style="5" customWidth="true"/>
-    <col min="6" max="6" width="5.77734375" style="5" customWidth="true"/>
-    <col min="7" max="7" width="3.109375" style="5" customWidth="true"/>
-    <col min="8" max="8" width="4.109375" style="5" customWidth="true"/>
-    <col min="9" max="9" width="3.6640625" style="5" customWidth="true"/>
-    <col min="10" max="10" width="12.6640625" style="5" customWidth="true"/>
-    <col min="11" max="11" width="2.109375" style="5" customWidth="true"/>
-    <col min="12" max="12" width="3.109375" style="5" customWidth="true"/>
-    <col min="13" max="13" width="5.109375" style="5" customWidth="true"/>
-    <col min="14" max="14" width="2.109375" style="5" customWidth="true"/>
-    <col min="15" max="15" width="5.109375" style="5" customWidth="true"/>
-    <col min="16" max="16" width="11.6640625" style="5" customWidth="true"/>
-    <col min="17" max="17" width="2.109375" style="5" customWidth="true"/>
-    <col min="18" max="18" width="11.6640625" style="5" bestFit="true" customWidth="true"/>
-    <col min="19" max="19" width="3.109375" style="2" customWidth="true"/>
-    <col min="20" max="20" width="11.6640625" style="2" customWidth="true"/>
-    <col min="21" max="21" width="7.6640625" style="2" customWidth="true"/>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="3.109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="2.109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="3.109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="2.109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="2.109375" style="5" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3971,7 +3968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -4039,7 +4036,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -4104,7 +4101,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4169,7 +4166,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -4234,7 +4231,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -4299,7 +4296,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -4364,7 +4361,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -4429,7 +4426,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -4494,7 +4491,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4559,7 +4556,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -4624,7 +4621,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -4689,7 +4686,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -4757,7 +4754,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -4822,7 +4819,7 @@
         <v>35027.99999999602</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -4884,7 +4881,7 @@
         <v>33599.399999997673</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -4949,7 +4946,7 @@
         <v>34393.39999999541</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5011,7 +5008,7 @@
         <v>34185.399999998022</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -5073,7 +5070,7 @@
         <v>44854.000000000749</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -5138,7 +5135,7 @@
         <v>41089.799999999734</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -5200,7 +5197,7 @@
         <v>33683.399999995439</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -5265,7 +5262,7 @@
         <v>38368.199999990931</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -5330,7 +5327,7 @@
         <v>29160.200000003344</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -5395,7 +5392,7 @@
         <v>26299.200000000703</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -5460,7 +5457,7 @@
         <v>35258.599999997146</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -5525,7 +5522,7 @@
         <v>38126.199999999233</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -5590,7 +5587,7 @@
         <v>41679.199999999524</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -5655,7 +5652,7 @@
         <v>37930.999999990832</v>
       </c>
     </row>
-    <row r="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -5717,7 +5714,7 @@
         <v>42732.199999994467</v>
       </c>
     </row>
-    <row r="29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -5782,7 +5779,7 @@
         <v>40585.200000000761</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -5847,7 +5844,7 @@
         <v>34076.799999998162</v>
       </c>
     </row>
-    <row r="31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -5909,7 +5906,7 @@
         <v>36910.599999998631</v>
       </c>
     </row>
-    <row r="32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -5971,7 +5968,7 @@
         <v>38119.400000000707</v>
       </c>
     </row>
-    <row r="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -6033,7 +6030,7 @@
         <v>36549.800000000418</v>
       </c>
     </row>
-    <row r="34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -6095,7 +6092,7 @@
         <v>33025.399999998008</v>
       </c>
     </row>
-    <row r="35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -6157,7 +6154,7 @@
         <v>35462.600000000064</v>
       </c>
     </row>
-    <row r="36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -6219,7 +6216,7 @@
         <v>31166.600000000191</v>
       </c>
     </row>
-    <row r="37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -6284,7 +6281,7 @@
         <v>36482.599999999664</v>
       </c>
     </row>
-    <row r="38" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -6349,7 +6346,7 @@
         <v>50976.800000001349</v>
       </c>
     </row>
-    <row r="39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -6411,7 +6408,7 @@
         <v>36606.399999994253</v>
       </c>
     </row>
-    <row r="40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -6476,7 +6473,7 @@
         <v>39421.000000000116</v>
       </c>
     </row>
-    <row r="41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -6541,7 +6538,7 @@
         <v>33620.00000000446</v>
       </c>
     </row>
-    <row r="42" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -6603,7 +6600,7 @@
         <v>30477.19999999983</v>
       </c>
     </row>
-    <row r="43" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -6665,7 +6662,7 @@
         <v>34542.999999999862</v>
       </c>
     </row>
-    <row r="44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -6727,7 +6724,7 @@
         <v>40761.199999999873</v>
       </c>
     </row>
-    <row r="45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>63</v>
       </c>
@@ -6790,7 +6787,7 @@
         <v>37345.599999996375</v>
       </c>
     </row>
-    <row r="46" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -6855,7 +6852,7 @@
         <v>33050.799999999683</v>
       </c>
     </row>
-    <row r="47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -6917,7 +6914,7 @@
         <v>35502.599999998631</v>
       </c>
     </row>
-    <row r="48" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -6979,7 +6976,7 @@
         <v>39358.799999999595</v>
       </c>
     </row>
-    <row r="49" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -7041,7 +7038,7 @@
         <v>30026.600000000013</v>
       </c>
     </row>
-    <row r="50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -7103,7 +7100,7 @@
         <v>33937.60000000037</v>
       </c>
     </row>
-    <row r="51" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -7165,7 +7162,7 @@
         <v>27155.000000000033</v>
       </c>
     </row>
-    <row r="52" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -7227,7 +7224,7 @@
         <v>30229.000000003762</v>
       </c>
     </row>
-    <row r="53" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -7292,7 +7289,7 @@
         <v>48978.399999997098</v>
       </c>
     </row>
-    <row r="54" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -7354,7 +7351,7 @@
         <v>30045.200000000623</v>
       </c>
     </row>
-    <row r="55" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -7416,7 +7413,7 @@
         <v>28900.599999999948</v>
       </c>
     </row>
-    <row r="56" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -7481,7 +7478,7 @@
         <v>38274.000000003412</v>
       </c>
     </row>
-    <row r="57" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -7546,7 +7543,7 @@
         <v>36662.599999997838</v>
       </c>
     </row>
-    <row r="58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -7611,7 +7608,7 @@
         <v>38512.200000000266</v>
       </c>
     </row>
-    <row r="59" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -7673,7 +7670,7 @@
         <v>29115.600000000741</v>
       </c>
     </row>
-    <row r="60" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -7738,7 +7735,7 @@
         <v>37488.000000001339</v>
       </c>
     </row>
-    <row r="61" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -7803,7 +7800,7 @@
         <v>38722.799999998148</v>
       </c>
     </row>
-    <row r="62" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -7868,7 +7865,7 @@
         <v>28778.400000005924</v>
       </c>
     </row>
-    <row r="63" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -7930,7 +7927,7 @@
         <v>27760.200000002103</v>
       </c>
     </row>
-    <row r="64" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -7995,7 +7992,7 @@
         <v>26513.400000003559</v>
       </c>
     </row>
-    <row r="65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -8057,7 +8054,7 @@
         <v>32324.20000000286</v>
       </c>
     </row>
-    <row r="66" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -8119,7 +8116,7 @@
         <v>22324.199999996672</v>
       </c>
     </row>
-    <row r="67" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -8184,7 +8181,7 @@
         <v>33364.60000000638</v>
       </c>
     </row>
-    <row r="68" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -8246,7 +8243,7 @@
         <v>30368.399999999674</v>
       </c>
     </row>
-    <row r="69" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -8308,7 +8305,7 @@
         <v>32919.799999997398</v>
       </c>
     </row>
-    <row r="70" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -8370,7 +8367,7 @@
         <v>32490.400000000889</v>
       </c>
     </row>
-    <row r="71" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>63</v>
       </c>
@@ -8435,7 +8432,7 @@
         <v>32790.800000001815</v>
       </c>
     </row>
-    <row r="72" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -8500,7 +8497,7 @@
         <v>32801.600000002523</v>
       </c>
     </row>
-    <row r="73" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>63</v>
       </c>
@@ -8596,29 +8593,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.48828125" customWidth="true"/>
-    <col min="2" max="2" width="8.26953125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="9.93359375" style="5" customWidth="true"/>
-    <col min="4" max="4" width="8.7109375" style="5" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="9.26953125" style="5" customWidth="true"/>
-    <col min="6" max="6" width="9.046875" style="5" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" style="5" customWidth="true"/>
-    <col min="8" max="8" width="12.046875" style="5" customWidth="true"/>
-    <col min="9" max="9" width="3.7109375" style="5" customWidth="true"/>
-    <col min="10" max="10" width="14.37890625" style="5" customWidth="true"/>
-    <col min="11" max="11" width="11.6015625" style="5" customWidth="true"/>
-    <col min="12" max="12" width="10.26953125" style="5" customWidth="true"/>
-    <col min="13" max="13" width="9.82421875" style="5" customWidth="true"/>
-    <col min="14" max="14" width="12.26953125" style="5" customWidth="true"/>
-    <col min="15" max="15" width="14.37890625" style="5" customWidth="true"/>
-    <col min="16" max="16" width="2.15625" style="5" customWidth="true"/>
-    <col min="17" max="17" width="11.7109375" style="5" bestFit="true" customWidth="true"/>
-    <col min="18" max="18" width="8.26953125" style="2" customWidth="true"/>
-    <col min="19" max="19" width="18.93359375" style="2" customWidth="true"/>
-    <col min="20" max="20" width="9.93359375" style="2" customWidth="true"/>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12" style="5" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="9.77734375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="2.109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.21875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="18.88671875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -8680,7 +8677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -8742,7 +8739,7 @@
         <v>29165.200000000514</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -8804,7 +8801,7 @@
         <v>32148.999999999323</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -8863,7 +8860,7 @@
         <v>28879.999999998843</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -8925,7 +8922,7 @@
         <v>29092.200000003271</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -8987,7 +8984,7 @@
         <v>29527.200000003089</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -9046,7 +9043,7 @@
         <v>26128.399999999743</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -9105,7 +9102,7 @@
         <v>36629.599999998638</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -9164,7 +9161,7 @@
         <v>29255.599999999486</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -9223,7 +9220,7 @@
         <v>32351.600000000621</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>119</v>
       </c>
@@ -9282,7 +9279,7 @@
         <v>37064.200000000121</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -9344,7 +9341,7 @@
         <v>35225.799999999879</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -9403,7 +9400,7 @@
         <v>32775.199999999699</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -9462,7 +9459,7 @@
         <v>42064.800000000119</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -9524,7 +9521,7 @@
         <v>42737.199999997887</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -9583,7 +9580,7 @@
         <v>43286.000000000298</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -9642,7 +9639,7 @@
         <v>48894.000000000153</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -9701,7 +9698,7 @@
         <v>39808.199999997771</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -9763,7 +9760,7 @@
         <v>43696.200000005461</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -9822,7 +9819,7 @@
         <v>33738.5999999954</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -9881,7 +9878,7 @@
         <v>39497.599999998303</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -9940,7 +9937,7 @@
         <v>30571.80000000216</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>119</v>
       </c>
@@ -9999,7 +9996,7 @@
         <v>40042.999999999811</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -10061,7 +10058,7 @@
         <v>37158.200000003693</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -10123,7 +10120,7 @@
         <v>43576.199999995697</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -10185,7 +10182,7 @@
         <v>55667.40000000225</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -10244,7 +10241,7 @@
         <v>34088.600000001556</v>
       </c>
     </row>
-    <row r="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -10303,7 +10300,7 @@
         <v>34135.199999999757</v>
       </c>
     </row>
-    <row r="29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -10365,7 +10362,7 @@
         <v>38286.199999988166</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -10424,7 +10421,7 @@
         <v>30056.200000001008</v>
       </c>
     </row>
-    <row r="31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -10483,7 +10480,7 @@
         <v>38416.799999997143</v>
       </c>
     </row>
-    <row r="32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -10545,7 +10542,7 @@
         <v>50684.199999990728</v>
       </c>
     </row>
-    <row r="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -10604,7 +10601,7 @@
         <v>40810.600000001854</v>
       </c>
     </row>
-    <row r="34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -10666,7 +10663,7 @@
         <v>49346.599999989463</v>
       </c>
     </row>
-    <row r="35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>119</v>
       </c>
@@ -10728,7 +10725,7 @@
         <v>43390.600000006285</v>
       </c>
     </row>
-    <row r="36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -10787,7 +10784,7 @@
         <v>30349.800000000203</v>
       </c>
     </row>
-    <row r="37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -10846,7 +10843,7 @@
         <v>39633.200000000492</v>
       </c>
     </row>
-    <row r="38" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -10905,7 +10902,7 @@
         <v>30935.800000001906</v>
       </c>
     </row>
-    <row r="39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -10964,7 +10961,7 @@
         <v>27782.60000000049</v>
       </c>
     </row>
-    <row r="40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -11023,7 +11020,7 @@
         <v>28711.399999999983</v>
       </c>
     </row>
-    <row r="41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -11082,7 +11079,7 @@
         <v>32224.199999999935</v>
       </c>
     </row>
-    <row r="42" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -11141,7 +11138,7 @@
         <v>24482.600000002334</v>
       </c>
     </row>
-    <row r="43" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -11200,7 +11197,7 @@
         <v>21468.800000000483</v>
       </c>
     </row>
-    <row r="44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>119</v>
       </c>
@@ -11262,7 +11259,7 @@
         <v>39340.599999995233</v>
       </c>
     </row>
-    <row r="45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>119</v>
       </c>
@@ -11324,7 +11321,7 @@
         <v>38564.999999998588</v>
       </c>
     </row>
-    <row r="46" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -11386,7 +11383,7 @@
         <v>40955.599999999824</v>
       </c>
     </row>
-    <row r="47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -11448,7 +11445,7 @@
         <v>33751.199999989847</v>
       </c>
     </row>
-    <row r="48" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -11510,7 +11507,7 @@
         <v>38959.999999998297</v>
       </c>
     </row>
-    <row r="49" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -11572,7 +11569,7 @@
         <v>37768.400000006339</v>
       </c>
     </row>
-    <row r="50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -11634,7 +11631,7 @@
         <v>31820.400000003734</v>
       </c>
     </row>
-    <row r="51" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -11693,7 +11690,7 @@
         <v>30756.000000000269</v>
       </c>
     </row>
-    <row r="52" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -11752,7 +11749,7 @@
         <v>28571.800000001876</v>
       </c>
     </row>
-    <row r="53" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>119</v>
       </c>
@@ -11811,7 +11808,7 @@
         <v>30477.199999999561</v>
       </c>
     </row>
-    <row r="54" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -11873,7 +11870,7 @@
         <v>31562.200000002707</v>
       </c>
     </row>
-    <row r="55" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -11932,7 +11929,7 @@
         <v>18789.4000000009</v>
       </c>
     </row>
-    <row r="56" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -11991,7 +11988,7 @@
         <v>34111.80000000068</v>
       </c>
     </row>
-    <row r="57" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -12050,7 +12047,7 @@
         <v>31760.200000002791</v>
       </c>
     </row>
-    <row r="58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -12112,7 +12109,7 @@
         <v>32771.400000002293</v>
       </c>
     </row>
-    <row r="59" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -12174,7 +12171,7 @@
         <v>32932.400000005939</v>
       </c>
     </row>
-    <row r="60" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -12236,7 +12233,7 @@
         <v>33675.199999998025</v>
       </c>
     </row>
-    <row r="61" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -12298,7 +12295,7 @@
         <v>30980.800000003019</v>
       </c>
     </row>
-    <row r="62" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -12357,7 +12354,7 @@
         <v>30653.400000000209</v>
       </c>
     </row>
-    <row r="63" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>179</v>
       </c>
@@ -12416,7 +12413,7 @@
         <v>30942.000000001513</v>
       </c>
     </row>
-    <row r="64" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>179</v>
       </c>
@@ -12475,7 +12472,7 @@
         <v>31707.200000002853</v>
       </c>
     </row>
-    <row r="65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>179</v>
       </c>
@@ -12534,7 +12531,7 @@
         <v>31359.600000003156</v>
       </c>
     </row>
-    <row r="66" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>179</v>
       </c>
@@ -12593,7 +12590,7 @@
         <v>31477.600000001203</v>
       </c>
     </row>
-    <row r="67" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -12652,7 +12649,7 @@
         <v>31041.999999999549</v>
       </c>
     </row>
-    <row r="68" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>186</v>
       </c>
@@ -12711,7 +12708,7 @@
         <v>33213.999999996209</v>
       </c>
     </row>
-    <row r="69" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>188</v>
       </c>
@@ -12773,7 +12770,7 @@
         <v>43995.00000000008</v>
       </c>
     </row>
-    <row r="70" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -12835,7 +12832,7 @@
         <v>38667.599999999715</v>
       </c>
     </row>
-    <row r="71" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>192</v>
       </c>
@@ -12894,7 +12891,7 @@
         <v>29930.399999998794</v>
       </c>
     </row>
-    <row r="72" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>194</v>
       </c>
@@ -12953,7 +12950,7 @@
         <v>28990.999999999593</v>
       </c>
     </row>
-    <row r="73" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>196</v>
       </c>
@@ -13013,7 +13010,7 @@
         <v>32166.199999998353</v>
       </c>
     </row>
-    <row r="74" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -13075,7 +13072,7 @@
         <v>43606.599999992613</v>
       </c>
     </row>
-    <row r="75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>200</v>
       </c>
@@ -13137,7 +13134,7 @@
         <v>42264.000000003056</v>
       </c>
     </row>
-    <row r="76" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>202</v>
       </c>
@@ -13199,7 +13196,7 @@
         <v>48968.799999999152</v>
       </c>
     </row>
-    <row r="77" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>204</v>
       </c>
@@ -13258,7 +13255,7 @@
         <v>9361.2000000002954</v>
       </c>
     </row>
-    <row r="78" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>206</v>
       </c>
@@ -13320,7 +13317,7 @@
         <v>10982.799999997991</v>
       </c>
     </row>
-    <row r="79" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>208</v>
       </c>
@@ -13382,24 +13379,24 @@
         <v>8193.999999999407</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>210</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>211</v>
       </c>
       <c r="C80" s="5">
         <v>1</v>
       </c>
       <c r="D80" s="5">
-        <v>9.9999999999999995e-07</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E80" s="5">
-        <v>1.0000000000000001e-20</v>
+        <v>1.0000000000000001E-20</v>
       </c>
       <c r="F80" s="5">
-        <v>1.0000000000000001e-21</v>
+        <v>1.0000000000000001E-21</v>
       </c>
       <c r="G80" s="5">
         <v>1000</v>
@@ -13408,10 +13405,10 @@
         <v>200</v>
       </c>
       <c r="I80" s="5">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J80" s="5">
-        <v>0.052359877559829883</v>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="K80" s="5">
         <v>24</v>
@@ -13444,24 +13441,24 @@
         <v>51456.400000001871</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>212</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>213</v>
       </c>
       <c r="C81" s="5">
         <v>1</v>
       </c>
       <c r="D81" s="5">
-        <v>9.9999999999999995e-07</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E81" s="5">
-        <v>1.0000000000000001e-20</v>
+        <v>1.0000000000000001E-20</v>
       </c>
       <c r="F81" s="5">
-        <v>1.0000000000000001e-21</v>
+        <v>1.0000000000000001E-21</v>
       </c>
       <c r="G81" s="5">
         <v>1000</v>
@@ -13470,10 +13467,10 @@
         <v>200</v>
       </c>
       <c r="I81" s="5">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J81" s="5">
-        <v>0.052359877559829883</v>
+        <v>5.2359877559829883E-2</v>
       </c>
       <c r="K81" s="5">
         <v>24</v>

</xml_diff>

<commit_message>
Minor changes to Swarm and my control functions
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEBB54A-3970-4CB0-B0E1-B1F5B387A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFAB8F7-4291-42F9-93B6-3F614B21C58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input (First Sheet Always)" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Log 06-29" sheetId="6" r:id="rId3"/>
     <sheet name="Log 06-30" sheetId="7" r:id="rId4"/>
     <sheet name="Log 07-01" sheetId="8" r:id="rId5"/>
+    <sheet name="Log 07-05" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="570">
   <si>
     <t>Sep</t>
   </si>
@@ -1587,6 +1588,162 @@
   </si>
   <si>
     <t>14:56:07</t>
+  </si>
+  <si>
+    <t>agentControl_Max</t>
+  </si>
+  <si>
+    <t>findNeighborhood_fixedRadius</t>
+  </si>
+  <si>
+    <t>07-05-22</t>
+  </si>
+  <si>
+    <t>09:12:27</t>
+  </si>
+  <si>
+    <t>agentControl_Max</t>
+  </si>
+  <si>
+    <t>findNeighborhood_fixedRadius</t>
+  </si>
+  <si>
+    <t>07-05-22</t>
+  </si>
+  <si>
+    <t>09:48:00</t>
+  </si>
+  <si>
+    <t>agentControl_Max</t>
+  </si>
+  <si>
+    <t>findNeighborhood_fixedRadius</t>
+  </si>
+  <si>
+    <t>07-05-22</t>
+  </si>
+  <si>
+    <t>09:57:46</t>
+  </si>
+  <si>
+    <t>09:58:34</t>
+  </si>
+  <si>
+    <t>09:56:22</t>
+  </si>
+  <si>
+    <t>09:57:54</t>
+  </si>
+  <si>
+    <t>09:56:54</t>
+  </si>
+  <si>
+    <t>09:57:36</t>
+  </si>
+  <si>
+    <t>agentControl_Max</t>
+  </si>
+  <si>
+    <t>findNeighborhood_fixedRadius</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>HCoh</t>
+  </si>
+  <si>
+    <t>HSep</t>
+  </si>
+  <si>
+    <t>Waggle</t>
+  </si>
+  <si>
+    <t>WaggleTime</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>TotalTime</t>
+  </si>
+  <si>
+    <t># Agents</t>
+  </si>
+  <si>
+    <t># Thermals</t>
+  </si>
+  <si>
+    <t>VisionRadius</t>
+  </si>
+  <si>
+    <t>FOV</t>
+  </si>
+  <si>
+    <t>CtrlFunction</t>
+  </si>
+  <si>
+    <t>NghbrFunction</t>
+  </si>
+  <si>
+    <t>MinSpeed</t>
+  </si>
+  <si>
+    <t>MaxSpeed</t>
+  </si>
+  <si>
+    <t>ThermStrMin</t>
+  </si>
+  <si>
+    <t>ThermStrMax</t>
+  </si>
+  <si>
+    <t>Survivors</t>
+  </si>
+  <si>
+    <t>AvgHeight</t>
+  </si>
+  <si>
+    <t>FlightTime</t>
+  </si>
+  <si>
+    <t>07-05-22</t>
+  </si>
+  <si>
+    <t>10:15:42</t>
+  </si>
+  <si>
+    <t>10:17:24</t>
+  </si>
+  <si>
+    <t>10:19:31</t>
+  </si>
+  <si>
+    <t>10:20:06</t>
+  </si>
+  <si>
+    <t>10:18:14</t>
+  </si>
+  <si>
+    <t>10:22:58</t>
   </si>
   <si>
     <t>agentControl_Max</t>
@@ -2098,6 +2255,41 @@
 </table>
 </file>
 
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E481E6B8-FE39-46BB-B479-5DDD7E0B7449}" name="Table5" displayName="Table5" ref="A1:Z15" totalsRowShown="0">
+  <autoFilter ref="A1:Z15" xr:uid="{E481E6B8-FE39-46BB-B479-5DDD7E0B7449}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{B9BBEB4D-B98C-4638-B71C-421A709AAF0D}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{F99EC8AA-FD27-4059-BC63-5454BEA0561C}" name="Time"/>
+    <tableColumn id="3" xr3:uid="{1E6E68B0-3140-4E3A-AB1A-42E01BA9110B}" name="S"/>
+    <tableColumn id="4" xr3:uid="{9C1E022E-B057-420D-8449-B082BB9A1121}" name="C"/>
+    <tableColumn id="5" xr3:uid="{E83DC47C-35ED-4DCB-87C2-988260EF758A}" name="A"/>
+    <tableColumn id="6" xr3:uid="{D75AB110-DD57-4E53-BC92-E47CFB8AD85D}" name="M"/>
+    <tableColumn id="7" xr3:uid="{7C515AFD-4A99-4BEE-8F7C-6166076ECD6B}" name="HCoh"/>
+    <tableColumn id="8" xr3:uid="{17FBBB79-554D-47B5-8DBF-6E96A0D8DC36}" name="HSep"/>
+    <tableColumn id="9" xr3:uid="{87724B4B-C096-4820-A51F-E6409AB73689}" name="Waggle"/>
+    <tableColumn id="10" xr3:uid="{2E121504-5C95-4CD3-91E2-8031B8073A20}" name="WaggleTime"/>
+    <tableColumn id="11" xr3:uid="{7DEFAC80-F2A3-4E1B-961C-A71D75DEA938}" name="K"/>
+    <tableColumn id="12" xr3:uid="{CA1923D6-D1E6-4C78-B08D-5FC9E47984C5}" name="dt"/>
+    <tableColumn id="13" xr3:uid="{B8E3A99E-9C4B-42A6-A975-2E6CC98E6C52}" name="TotalTime"/>
+    <tableColumn id="14" xr3:uid="{25F81FB4-6F27-4C66-903E-EE07D257F941}" name="# Agents"/>
+    <tableColumn id="15" xr3:uid="{9E2FC01D-F1EA-46BE-A9AE-BAD2C5B3A17B}" name="# Thermals"/>
+    <tableColumn id="16" xr3:uid="{184AEB26-0308-45AF-9BA1-6A0BDA8EA839}" name="VisionRadius"/>
+    <tableColumn id="17" xr3:uid="{760A08BE-6813-4022-A1EF-CD731FF6AB70}" name="FOV"/>
+    <tableColumn id="18" xr3:uid="{F4C5D401-C802-47D5-A9A8-50999854E30D}" name="CtrlFunction"/>
+    <tableColumn id="19" xr3:uid="{5FF7CBE1-C19C-47D3-8440-433C7A58B3AA}" name="NghbrFunction"/>
+    <tableColumn id="20" xr3:uid="{E5D55891-5493-4DB5-B9DF-4CD2E56FF798}" name="MinSpeed"/>
+    <tableColumn id="21" xr3:uid="{22F0A8A8-0399-4E4E-9A89-866857D838BB}" name="MaxSpeed"/>
+    <tableColumn id="22" xr3:uid="{953E8247-8BFE-4C91-BE80-F4759E99C80C}" name="ThermStrMin"/>
+    <tableColumn id="23" xr3:uid="{89B923F2-A863-496B-B780-ACDEC6E7D96F}" name="ThermStrMax"/>
+    <tableColumn id="24" xr3:uid="{32429B91-157F-498C-AC92-01D8E730DFA9}" name="Survivors"/>
+    <tableColumn id="25" xr3:uid="{BF213A3E-335D-464A-B513-9D2D8D64A978}" name="AvgHeight"/>
+    <tableColumn id="26" xr3:uid="{A693EF48-267E-4D97-B632-15896ECA100C}" name="FlightTime"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2397,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,7 +2704,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C2" s="21">
         <v>-4</v>
@@ -2524,7 +2716,7 @@
         <v>-21</v>
       </c>
       <c r="F2" s="6">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5">
         <v>200</v>
@@ -2595,7 +2787,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C3" s="21">
         <v>-4</v>
@@ -2607,7 +2799,7 @@
         <v>-21</v>
       </c>
       <c r="F3" s="6">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5">
         <v>200</v>
@@ -2678,7 +2870,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C4" s="21">
         <v>-4</v>
@@ -2690,7 +2882,7 @@
         <v>-21</v>
       </c>
       <c r="F4" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5">
         <v>200</v>
@@ -2761,19 +2953,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C5" s="21">
         <v>-4</v>
       </c>
       <c r="D5" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E5" s="5">
         <v>-21</v>
       </c>
       <c r="F5" s="6">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="G5" s="5">
         <v>200</v>
@@ -2847,19 +3039,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C6" s="21">
         <v>-4</v>
       </c>
       <c r="D6" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E6" s="5">
         <v>-21</v>
       </c>
       <c r="F6" s="6">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="G6" s="5">
         <v>200</v>
@@ -2930,19 +3122,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C7" s="21">
         <v>-4</v>
       </c>
       <c r="D7" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E7" s="5">
         <v>-21</v>
       </c>
       <c r="F7" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G7" s="5">
         <v>200</v>
@@ -3015,48 +3207,20 @@
       <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D8" s="5">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F8" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G8" s="5">
-        <v>200</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>40</v>
-      </c>
-      <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
-        <v>10</v>
-      </c>
-      <c r="N8" s="5">
-        <v>8</v>
-      </c>
-      <c r="O8" s="5">
-        <v>13</v>
-      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
       <c r="Q8">
         <v>6</v>
       </c>
@@ -3098,48 +3262,20 @@
       <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2</v>
-      </c>
-      <c r="E9" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G9" s="5">
-        <v>200</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>40</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
-        <v>10</v>
-      </c>
-      <c r="N9" s="5">
-        <v>8</v>
-      </c>
-      <c r="O9" s="5">
-        <v>13</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
       <c r="Q9">
         <v>4</v>
       </c>
@@ -3184,48 +3320,20 @@
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F10" s="6">
-        <v>100</v>
-      </c>
-      <c r="G10" s="5">
-        <v>200</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>40</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
-        <v>10</v>
-      </c>
-      <c r="N10" s="5">
-        <v>8</v>
-      </c>
-      <c r="O10" s="5">
-        <v>13</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
@@ -3233,48 +3341,20 @@
       <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
-        <v>2</v>
-      </c>
-      <c r="C11" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D11" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E11" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F11" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G11" s="5">
-        <v>200</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>40</v>
-      </c>
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5">
-        <v>10</v>
-      </c>
-      <c r="N11" s="5">
-        <v>8</v>
-      </c>
-      <c r="O11" s="5">
-        <v>13</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
@@ -3282,48 +3362,20 @@
       <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
-        <v>2</v>
-      </c>
-      <c r="C12" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D12" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E12" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G12" s="5">
-        <v>200</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>40</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5">
-        <v>10</v>
-      </c>
-      <c r="N12" s="5">
-        <v>8</v>
-      </c>
-      <c r="O12" s="5">
-        <v>13</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
@@ -3331,48 +3383,20 @@
       <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
-        <v>2</v>
-      </c>
-      <c r="C13" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D13" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E13" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F13" s="6">
-        <v>100</v>
-      </c>
-      <c r="G13" s="5">
-        <v>200</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0</v>
-      </c>
-      <c r="K13" s="5">
-        <v>40</v>
-      </c>
-      <c r="L13" s="5">
-        <v>1</v>
-      </c>
-      <c r="M13" s="5">
-        <v>10</v>
-      </c>
-      <c r="N13" s="5">
-        <v>8</v>
-      </c>
-      <c r="O13" s="5">
-        <v>13</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
@@ -3380,48 +3404,20 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F14" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G14" s="5">
-        <v>200</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
-        <v>40</v>
-      </c>
-      <c r="L14" s="5">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <v>10</v>
-      </c>
-      <c r="N14" s="5">
-        <v>8</v>
-      </c>
-      <c r="O14" s="5">
-        <v>13</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
@@ -3429,48 +3425,20 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G15" s="5">
-        <v>200</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>40</v>
-      </c>
-      <c r="L15" s="5">
-        <v>1</v>
-      </c>
-      <c r="M15" s="5">
-        <v>10</v>
-      </c>
-      <c r="N15" s="5">
-        <v>8</v>
-      </c>
-      <c r="O15" s="5">
-        <v>13</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
@@ -3478,48 +3446,20 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
-        <v>2</v>
-      </c>
-      <c r="C16" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F16" s="6">
-        <v>100</v>
-      </c>
-      <c r="G16" s="5">
-        <v>200</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <v>40</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1</v>
-      </c>
-      <c r="M16" s="5">
-        <v>10</v>
-      </c>
-      <c r="N16" s="5">
-        <v>8</v>
-      </c>
-      <c r="O16" s="5">
-        <v>13</v>
-      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
@@ -3527,565 +3467,229 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
-        <v>2</v>
-      </c>
-      <c r="C17" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2</v>
-      </c>
-      <c r="E17" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F17" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G17" s="5">
-        <v>200</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>40</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5">
-        <v>10</v>
-      </c>
-      <c r="N17" s="5">
-        <v>8</v>
-      </c>
-      <c r="O17" s="5">
-        <v>13</v>
-      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="5">
-        <v>2</v>
-      </c>
-      <c r="C18" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G18" s="5">
-        <v>200</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
-        <v>40</v>
-      </c>
-      <c r="L18" s="5">
-        <v>1</v>
-      </c>
-      <c r="M18" s="5">
-        <v>10</v>
-      </c>
-      <c r="N18" s="5">
-        <v>8</v>
-      </c>
-      <c r="O18" s="5">
-        <v>13</v>
-      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="5">
-        <v>2</v>
-      </c>
-      <c r="C19" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2</v>
-      </c>
-      <c r="E19" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F19" s="6">
-        <v>100</v>
-      </c>
-      <c r="G19" s="5">
-        <v>200</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
-        <v>40</v>
-      </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5">
-        <v>10</v>
-      </c>
-      <c r="N19" s="5">
-        <v>8</v>
-      </c>
-      <c r="O19" s="5">
-        <v>13</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C20" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D20" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E20" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F20" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G20" s="5">
-        <v>200</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I20" s="5">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
-        <v>40</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1</v>
-      </c>
-      <c r="M20" s="5">
-        <v>10</v>
-      </c>
-      <c r="N20" s="5">
-        <v>8</v>
-      </c>
-      <c r="O20" s="5">
-        <v>13</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C21" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D21" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E21" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G21" s="5">
-        <v>200</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5">
-        <v>40</v>
-      </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5">
-        <v>10</v>
-      </c>
-      <c r="N21" s="5">
-        <v>8</v>
-      </c>
-      <c r="O21" s="5">
-        <v>13</v>
-      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C22" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D22" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E22" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F22" s="6">
-        <v>100</v>
-      </c>
-      <c r="G22" s="5">
-        <v>200</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <v>40</v>
-      </c>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5">
-        <v>10</v>
-      </c>
-      <c r="N22" s="5">
-        <v>8</v>
-      </c>
-      <c r="O22" s="5">
-        <v>13</v>
-      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C23" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F23" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G23" s="5">
-        <v>200</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
-        <v>40</v>
-      </c>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
-      <c r="M23" s="5">
-        <v>10</v>
-      </c>
-      <c r="N23" s="5">
-        <v>8</v>
-      </c>
-      <c r="O23" s="5">
-        <v>13</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C24" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G24" s="5">
-        <v>200</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I24" s="5">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5">
-        <v>0</v>
-      </c>
-      <c r="K24" s="5">
-        <v>40</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5">
-        <v>10</v>
-      </c>
-      <c r="N24" s="5">
-        <v>8</v>
-      </c>
-      <c r="O24" s="5">
-        <v>13</v>
-      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>24</v>
       </c>
-      <c r="B25" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C25" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F25" s="6">
-        <v>100</v>
-      </c>
-      <c r="G25" s="5">
-        <v>200</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5">
-        <v>40</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="5">
-        <v>10</v>
-      </c>
-      <c r="N25" s="5">
-        <v>8</v>
-      </c>
-      <c r="O25" s="5">
-        <v>13</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C26" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D26" s="5">
-        <v>2</v>
-      </c>
-      <c r="E26" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F26" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G26" s="5">
-        <v>200</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I26" s="5">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5">
-        <v>40</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5">
-        <v>10</v>
-      </c>
-      <c r="N26" s="5">
-        <v>8</v>
-      </c>
-      <c r="O26" s="5">
-        <v>13</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C27" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D27" s="5">
-        <v>2</v>
-      </c>
-      <c r="E27" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G27" s="5">
-        <v>200</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>0</v>
-      </c>
-      <c r="K27" s="5">
-        <v>40</v>
-      </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5">
-        <v>10</v>
-      </c>
-      <c r="N27" s="5">
-        <v>8</v>
-      </c>
-      <c r="O27" s="5">
-        <v>13</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="5">
-        <v>-2</v>
-      </c>
-      <c r="C28" s="21">
-        <v>-4</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2</v>
-      </c>
-      <c r="E28" s="5">
-        <v>-21</v>
-      </c>
-      <c r="F28" s="6">
-        <v>100</v>
-      </c>
-      <c r="G28" s="5">
-        <v>200</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I28" s="5">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5">
-        <v>0</v>
-      </c>
-      <c r="K28" s="5">
-        <v>40</v>
-      </c>
-      <c r="L28" s="5">
-        <v>1</v>
-      </c>
-      <c r="M28" s="5">
-        <v>10</v>
-      </c>
-      <c r="N28" s="5">
-        <v>8</v>
-      </c>
-      <c r="O28" s="5">
-        <v>13</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
@@ -26260,8 +25864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J20" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30134,4 +29738,1254 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:Z15"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9:X15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" customWidth="1"/>
+    <col min="9" max="10" width="2.109375" customWidth="1"/>
+    <col min="11" max="11" width="3.109375" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" customWidth="1"/>
+    <col min="14" max="14" width="3.109375" customWidth="1"/>
+    <col min="15" max="15" width="2.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.109375" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" customWidth="1"/>
+    <col min="19" max="19" width="26.21875" customWidth="1"/>
+    <col min="20" max="20" width="2.109375" customWidth="1"/>
+    <col min="21" max="21" width="3.109375" customWidth="1"/>
+    <col min="22" max="22" width="2.109375" customWidth="1"/>
+    <col min="23" max="24" width="3.109375" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" customWidth="1"/>
+    <col min="26" max="26" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E1" t="s">
+        <v>539</v>
+      </c>
+      <c r="F1" t="s">
+        <v>540</v>
+      </c>
+      <c r="G1" t="s">
+        <v>541</v>
+      </c>
+      <c r="H1" t="s">
+        <v>542</v>
+      </c>
+      <c r="I1" t="s">
+        <v>543</v>
+      </c>
+      <c r="J1" t="s">
+        <v>544</v>
+      </c>
+      <c r="K1" t="s">
+        <v>545</v>
+      </c>
+      <c r="L1" t="s">
+        <v>546</v>
+      </c>
+      <c r="M1" t="s">
+        <v>547</v>
+      </c>
+      <c r="N1" t="s">
+        <v>548</v>
+      </c>
+      <c r="O1" t="s">
+        <v>549</v>
+      </c>
+      <c r="P1" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>551</v>
+      </c>
+      <c r="R1" t="s">
+        <v>552</v>
+      </c>
+      <c r="S1" t="s">
+        <v>553</v>
+      </c>
+      <c r="T1" t="s">
+        <v>554</v>
+      </c>
+      <c r="U1" t="s">
+        <v>555</v>
+      </c>
+      <c r="V1" t="s">
+        <v>556</v>
+      </c>
+      <c r="W1" t="s">
+        <v>557</v>
+      </c>
+      <c r="X1" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>559</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>1E-4</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+      <c r="F2">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>0.2</v>
+      </c>
+      <c r="M2">
+        <v>5400</v>
+      </c>
+      <c r="N2">
+        <v>40</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>4000</v>
+      </c>
+      <c r="Q2">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R2" t="s">
+        <v>520</v>
+      </c>
+      <c r="S2" t="s">
+        <v>521</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>13</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>40</v>
+      </c>
+      <c r="Y2">
+        <v>2404.8612535680277</v>
+      </c>
+      <c r="Z2">
+        <v>216000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>522</v>
+      </c>
+      <c r="B3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>1E-4</v>
+      </c>
+      <c r="E3">
+        <v>0.01</v>
+      </c>
+      <c r="F3">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>0.2</v>
+      </c>
+      <c r="M3">
+        <v>5400</v>
+      </c>
+      <c r="N3">
+        <v>40</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>4000</v>
+      </c>
+      <c r="Q3">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R3" t="s">
+        <v>524</v>
+      </c>
+      <c r="S3" t="s">
+        <v>525</v>
+      </c>
+      <c r="T3">
+        <v>8</v>
+      </c>
+      <c r="U3">
+        <v>13</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>10</v>
+      </c>
+      <c r="X3">
+        <v>40</v>
+      </c>
+      <c r="Y3">
+        <v>2214.9296766900588</v>
+      </c>
+      <c r="Z3">
+        <v>216000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>526</v>
+      </c>
+      <c r="B4" t="s">
+        <v>527</v>
+      </c>
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>1E-4</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G4">
+        <v>10000</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>0.2</v>
+      </c>
+      <c r="M4">
+        <v>5400</v>
+      </c>
+      <c r="N4">
+        <v>40</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>4000</v>
+      </c>
+      <c r="Q4">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R4" t="s">
+        <v>533</v>
+      </c>
+      <c r="S4" t="s">
+        <v>534</v>
+      </c>
+      <c r="T4">
+        <v>8</v>
+      </c>
+      <c r="U4">
+        <v>13</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>10</v>
+      </c>
+      <c r="X4">
+        <v>6</v>
+      </c>
+      <c r="Y4">
+        <v>2477.5974853306029</v>
+      </c>
+      <c r="Z4">
+        <v>70923.199999971461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B5" t="s">
+        <v>528</v>
+      </c>
+      <c r="C5">
+        <v>0.01</v>
+      </c>
+      <c r="D5">
+        <v>1E-4</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G5">
+        <v>10000</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>0.2</v>
+      </c>
+      <c r="M5">
+        <v>5400</v>
+      </c>
+      <c r="N5">
+        <v>40</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>4000</v>
+      </c>
+      <c r="Q5">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R5" t="s">
+        <v>533</v>
+      </c>
+      <c r="S5" t="s">
+        <v>534</v>
+      </c>
+      <c r="T5">
+        <v>8</v>
+      </c>
+      <c r="U5">
+        <v>13</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>10</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>86978.200000013559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>526</v>
+      </c>
+      <c r="B6" t="s">
+        <v>529</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>1E-4</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G6">
+        <v>10000</v>
+      </c>
+      <c r="H6">
+        <v>200</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>0.2</v>
+      </c>
+      <c r="M6">
+        <v>5400</v>
+      </c>
+      <c r="N6">
+        <v>40</v>
+      </c>
+      <c r="O6">
+        <v>6</v>
+      </c>
+      <c r="P6">
+        <v>4000</v>
+      </c>
+      <c r="Q6">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R6" t="s">
+        <v>533</v>
+      </c>
+      <c r="S6" t="s">
+        <v>534</v>
+      </c>
+      <c r="T6">
+        <v>8</v>
+      </c>
+      <c r="U6">
+        <v>13</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>10</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>28.398714692514883</v>
+      </c>
+      <c r="Z6">
+        <v>30029.200000027049</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B7" t="s">
+        <v>530</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>1E-4</v>
+      </c>
+      <c r="E7">
+        <v>0.01</v>
+      </c>
+      <c r="F7">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G7">
+        <v>10000</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>0.2</v>
+      </c>
+      <c r="M7">
+        <v>5400</v>
+      </c>
+      <c r="N7">
+        <v>40</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>4000</v>
+      </c>
+      <c r="Q7">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R7" t="s">
+        <v>533</v>
+      </c>
+      <c r="S7" t="s">
+        <v>534</v>
+      </c>
+      <c r="T7">
+        <v>8</v>
+      </c>
+      <c r="U7">
+        <v>13</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>10</v>
+      </c>
+      <c r="X7">
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <v>1079.4265882556297</v>
+      </c>
+      <c r="Z7">
+        <v>68781.200000006793</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>526</v>
+      </c>
+      <c r="B8" t="s">
+        <v>531</v>
+      </c>
+      <c r="C8">
+        <v>0.01</v>
+      </c>
+      <c r="D8">
+        <v>1E-4</v>
+      </c>
+      <c r="E8">
+        <v>0.01</v>
+      </c>
+      <c r="F8">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G8">
+        <v>10000</v>
+      </c>
+      <c r="H8">
+        <v>200</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>0.2</v>
+      </c>
+      <c r="M8">
+        <v>5400</v>
+      </c>
+      <c r="N8">
+        <v>40</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>4000</v>
+      </c>
+      <c r="Q8">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R8" t="s">
+        <v>533</v>
+      </c>
+      <c r="S8" t="s">
+        <v>534</v>
+      </c>
+      <c r="T8">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <v>13</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>523.08706078763259</v>
+      </c>
+      <c r="Z8">
+        <v>40037.600000027312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>526</v>
+      </c>
+      <c r="B9" t="s">
+        <v>532</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>1E-4</v>
+      </c>
+      <c r="E9">
+        <v>0.01</v>
+      </c>
+      <c r="F9">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G9">
+        <v>10000</v>
+      </c>
+      <c r="H9">
+        <v>200</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <v>0.2</v>
+      </c>
+      <c r="M9">
+        <v>5400</v>
+      </c>
+      <c r="N9">
+        <v>40</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>4000</v>
+      </c>
+      <c r="Q9">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R9" t="s">
+        <v>533</v>
+      </c>
+      <c r="S9" t="s">
+        <v>534</v>
+      </c>
+      <c r="T9">
+        <v>8</v>
+      </c>
+      <c r="U9">
+        <v>13</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>10</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>59271.99999996354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>561</v>
+      </c>
+      <c r="B10" t="s">
+        <v>562</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+      <c r="D10">
+        <v>1E-4</v>
+      </c>
+      <c r="E10">
+        <v>0.01</v>
+      </c>
+      <c r="F10">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G10">
+        <v>10000</v>
+      </c>
+      <c r="H10">
+        <v>200</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>0.2</v>
+      </c>
+      <c r="M10">
+        <v>5400</v>
+      </c>
+      <c r="N10">
+        <v>40</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>4000</v>
+      </c>
+      <c r="Q10">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R10" t="s">
+        <v>568</v>
+      </c>
+      <c r="S10" t="s">
+        <v>569</v>
+      </c>
+      <c r="T10">
+        <v>8</v>
+      </c>
+      <c r="U10">
+        <v>13</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>10</v>
+      </c>
+      <c r="X10">
+        <v>12</v>
+      </c>
+      <c r="Y10">
+        <v>2600</v>
+      </c>
+      <c r="Z10">
+        <v>104404.3999999761</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>561</v>
+      </c>
+      <c r="B11" t="s">
+        <v>563</v>
+      </c>
+      <c r="C11">
+        <v>0.01</v>
+      </c>
+      <c r="D11">
+        <v>1E-4</v>
+      </c>
+      <c r="E11">
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>200</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>0.2</v>
+      </c>
+      <c r="M11">
+        <v>5400</v>
+      </c>
+      <c r="N11">
+        <v>40</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <v>4000</v>
+      </c>
+      <c r="Q11">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R11" t="s">
+        <v>568</v>
+      </c>
+      <c r="S11" t="s">
+        <v>569</v>
+      </c>
+      <c r="T11">
+        <v>8</v>
+      </c>
+      <c r="U11">
+        <v>13</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>10</v>
+      </c>
+      <c r="X11">
+        <v>14</v>
+      </c>
+      <c r="Y11">
+        <v>2447.1227592282044</v>
+      </c>
+      <c r="Z11">
+        <v>125468.00000001949</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>561</v>
+      </c>
+      <c r="B12" t="s">
+        <v>564</v>
+      </c>
+      <c r="C12">
+        <v>0.01</v>
+      </c>
+      <c r="D12">
+        <v>1E-4</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+      <c r="F12">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G12">
+        <v>10000</v>
+      </c>
+      <c r="H12">
+        <v>200</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>0.2</v>
+      </c>
+      <c r="M12">
+        <v>5400</v>
+      </c>
+      <c r="N12">
+        <v>40</v>
+      </c>
+      <c r="O12">
+        <v>6</v>
+      </c>
+      <c r="P12">
+        <v>4000</v>
+      </c>
+      <c r="Q12">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R12" t="s">
+        <v>568</v>
+      </c>
+      <c r="S12" t="s">
+        <v>569</v>
+      </c>
+      <c r="T12">
+        <v>8</v>
+      </c>
+      <c r="U12">
+        <v>13</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>10</v>
+      </c>
+      <c r="X12">
+        <v>16</v>
+      </c>
+      <c r="Y12">
+        <v>2591.5254287868247</v>
+      </c>
+      <c r="Z12">
+        <v>157968.00000006796</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>561</v>
+      </c>
+      <c r="B13" t="s">
+        <v>565</v>
+      </c>
+      <c r="C13">
+        <v>0.01</v>
+      </c>
+      <c r="D13">
+        <v>1E-4</v>
+      </c>
+      <c r="E13">
+        <v>0.01</v>
+      </c>
+      <c r="F13">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G13">
+        <v>10000</v>
+      </c>
+      <c r="H13">
+        <v>200</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <v>0.2</v>
+      </c>
+      <c r="M13">
+        <v>5400</v>
+      </c>
+      <c r="N13">
+        <v>40</v>
+      </c>
+      <c r="O13">
+        <v>6</v>
+      </c>
+      <c r="P13">
+        <v>4000</v>
+      </c>
+      <c r="Q13">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R13" t="s">
+        <v>568</v>
+      </c>
+      <c r="S13" t="s">
+        <v>569</v>
+      </c>
+      <c r="T13">
+        <v>8</v>
+      </c>
+      <c r="U13">
+        <v>13</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>10</v>
+      </c>
+      <c r="X13">
+        <v>28</v>
+      </c>
+      <c r="Y13">
+        <v>2331.8761374868677</v>
+      </c>
+      <c r="Z13">
+        <v>169508.40000010672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B14" t="s">
+        <v>566</v>
+      </c>
+      <c r="C14">
+        <v>0.01</v>
+      </c>
+      <c r="D14">
+        <v>1E-4</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G14">
+        <v>10000</v>
+      </c>
+      <c r="H14">
+        <v>200</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>0.2</v>
+      </c>
+      <c r="M14">
+        <v>5400</v>
+      </c>
+      <c r="N14">
+        <v>40</v>
+      </c>
+      <c r="O14">
+        <v>6</v>
+      </c>
+      <c r="P14">
+        <v>4000</v>
+      </c>
+      <c r="Q14">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R14" t="s">
+        <v>568</v>
+      </c>
+      <c r="S14" t="s">
+        <v>569</v>
+      </c>
+      <c r="T14">
+        <v>8</v>
+      </c>
+      <c r="U14">
+        <v>13</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>10</v>
+      </c>
+      <c r="X14">
+        <v>18</v>
+      </c>
+      <c r="Y14">
+        <v>1859.2586175915219</v>
+      </c>
+      <c r="Z14">
+        <v>140998.80000007764</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>561</v>
+      </c>
+      <c r="B15" t="s">
+        <v>567</v>
+      </c>
+      <c r="C15">
+        <v>0.01</v>
+      </c>
+      <c r="D15">
+        <v>1E-4</v>
+      </c>
+      <c r="E15">
+        <v>0.01</v>
+      </c>
+      <c r="F15">
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="G15">
+        <v>10000</v>
+      </c>
+      <c r="H15">
+        <v>200</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>0.2</v>
+      </c>
+      <c r="M15">
+        <v>5400</v>
+      </c>
+      <c r="N15">
+        <v>40</v>
+      </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
+      <c r="P15">
+        <v>4000</v>
+      </c>
+      <c r="Q15">
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="R15" t="s">
+        <v>568</v>
+      </c>
+      <c r="S15" t="s">
+        <v>569</v>
+      </c>
+      <c r="T15">
+        <v>8</v>
+      </c>
+      <c r="U15">
+        <v>13</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+      <c r="X15">
+        <v>32</v>
+      </c>
+      <c r="Y15">
+        <v>2436.6579501952838</v>
+      </c>
+      <c r="Z15">
+        <v>208718.80000005642</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="Z2:Z15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
attempt made for adding ToD to swarm
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED22B486-AC8F-4830-8629-C201973AE12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DFFFA9-5A94-43D4-9AFD-7ED9151A43D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input (First Sheet Always)" sheetId="2" r:id="rId1"/>
@@ -2664,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331EDB9E-F266-4673-92BF-7340BFE1C794}">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2788,7 +2788,7 @@
         <v>-2</v>
       </c>
       <c r="E2" s="5">
-        <v>-21</v>
+        <v>-23</v>
       </c>
       <c r="F2" s="6">
         <v>10</v>
@@ -29875,7 +29875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K14" workbookViewId="0">
+    <sheetView topLeftCell="K14" workbookViewId="0">
       <selection activeCell="Y31" sqref="Y31"/>
     </sheetView>
   </sheetViews>

</xml_diff>